<commit_message>
Neo supplied updated mapping of Group C comorbidity categories
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2822" uniqueCount="579">
   <si>
     <t>coding</t>
   </si>
@@ -1602,9 +1602,6 @@
     <t>chronic respiratory disease</t>
   </si>
   <si>
-    <t>neurological</t>
-  </si>
-  <si>
     <t>other back problem</t>
   </si>
   <si>
@@ -1614,9 +1611,6 @@
     <t>arthiritis (nos)</t>
   </si>
   <si>
-    <t>dupuytren's contractture</t>
-  </si>
-  <si>
     <t>musculoskeletal- chronic pain</t>
   </si>
   <si>
@@ -1711,6 +1705,60 @@
   </si>
   <si>
     <t>Group B</t>
+  </si>
+  <si>
+    <t>(blank, no longer categorized as stroke) - no longer in the grouping because technically not a chronic condition</t>
+  </si>
+  <si>
+    <t>Endo - thyroid disorder</t>
+  </si>
+  <si>
+    <t>hyperthyroidism</t>
+  </si>
+  <si>
+    <t>hypothyroidism</t>
+  </si>
+  <si>
+    <t>goiter</t>
+  </si>
+  <si>
+    <t>thyroid problem nos</t>
+  </si>
+  <si>
+    <t>leave blank - note that removed from morbidity groupings</t>
+  </si>
+  <si>
+    <t>eating disorder</t>
+  </si>
+  <si>
+    <t>other psychological/psychiatric problem</t>
+  </si>
+  <si>
+    <t>Neurological</t>
+  </si>
+  <si>
+    <t>ComorbidityType</t>
+  </si>
+  <si>
+    <t>Other cardiac</t>
+  </si>
+  <si>
+    <t>Musculoskeletal - chronic pain</t>
+  </si>
+  <si>
+    <t>Chronic Respiratory Disease</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>NB. including cardiomyopathy as one of the comorbidity diagnoses in Group C</t>
+  </si>
+  <si>
+    <t>Connective Tissue Disorder</t>
+  </si>
+  <si>
+    <t>Communicable Disease</t>
   </si>
 </sst>
 </file>
@@ -2230,7 +2278,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2243,6 +2291,15 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2596,11 +2653,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L447"/>
+  <dimension ref="A1:N447"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L258" sqref="L258"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L377" sqref="L377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,10 +2671,11 @@
     <col min="9" max="10" width="17" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2649,13 +2707,19 @@
         <v>521</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1425</v>
       </c>
@@ -2675,7 +2739,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1491</v>
       </c>
@@ -2701,13 +2765,16 @@
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1583</v>
       </c>
@@ -2733,13 +2800,16 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1086</v>
       </c>
@@ -2765,13 +2835,16 @@
         <v>9</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1081</v>
       </c>
@@ -2794,13 +2867,16 @@
         <v>9</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1083</v>
       </c>
@@ -2819,17 +2895,11 @@
       <c r="H7" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1082</v>
       </c>
@@ -2852,13 +2922,16 @@
         <v>9</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1074</v>
       </c>
@@ -2881,13 +2954,16 @@
         <v>522</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1588</v>
       </c>
@@ -2913,10 +2989,19 @@
         <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1079</v>
       </c>
@@ -2939,10 +3024,16 @@
         <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1471</v>
       </c>
@@ -2965,16 +3056,19 @@
         <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1483</v>
       </c>
@@ -2997,16 +3091,19 @@
         <v>19</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1485</v>
       </c>
@@ -3029,13 +3126,13 @@
         <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1486</v>
       </c>
@@ -3058,13 +3155,13 @@
         <v>19</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1487</v>
       </c>
@@ -3087,13 +3184,13 @@
         <v>19</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1484</v>
       </c>
@@ -3116,13 +3213,13 @@
         <v>19</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1077</v>
       </c>
@@ -3142,13 +3239,13 @@
         <v>19</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1075</v>
       </c>
@@ -3171,13 +3268,16 @@
         <v>522</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1076</v>
       </c>
@@ -3200,13 +3300,13 @@
         <v>517</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1587</v>
       </c>
@@ -3235,10 +3335,16 @@
         <v>484</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1490</v>
       </c>
@@ -3267,10 +3373,16 @@
         <v>484</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1586</v>
       </c>
@@ -3296,10 +3408,16 @@
         <v>484</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1585</v>
       </c>
@@ -3328,10 +3446,16 @@
         <v>484</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1489</v>
       </c>
@@ -3360,10 +3484,16 @@
         <v>484</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1488</v>
       </c>
@@ -3392,10 +3522,16 @@
         <v>484</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1584</v>
       </c>
@@ -3421,10 +3557,16 @@
         <v>484</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1078</v>
       </c>
@@ -3447,10 +3589,16 @@
         <v>484</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1426</v>
       </c>
@@ -3473,10 +3621,16 @@
         <v>36</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1590</v>
       </c>
@@ -3502,10 +3656,16 @@
         <v>38</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1589</v>
       </c>
@@ -3531,10 +3691,16 @@
         <v>39</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1080</v>
       </c>
@@ -3557,10 +3723,16 @@
         <v>37</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1479</v>
       </c>
@@ -3583,10 +3755,10 @@
         <v>40</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1066</v>
       </c>
@@ -3603,13 +3775,19 @@
         <v>519</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1473</v>
       </c>
@@ -3629,10 +3807,16 @@
         <v>41</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1072</v>
       </c>
@@ -3652,7 +3836,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1073</v>
       </c>
@@ -3672,7 +3856,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1065</v>
       </c>
@@ -3689,7 +3873,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1495</v>
       </c>
@@ -3712,10 +3896,16 @@
         <v>46</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1593</v>
       </c>
@@ -3735,7 +3925,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1494</v>
       </c>
@@ -3755,7 +3945,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1493</v>
       </c>
@@ -3772,7 +3962,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1591</v>
       </c>
@@ -3794,8 +3984,21 @@
       <c r="H43" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>1592</v>
       </c>
@@ -3817,8 +4020,21 @@
       <c r="H44" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1492</v>
       </c>
@@ -3837,8 +4053,21 @@
       <c r="H45" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I45" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1088</v>
       </c>
@@ -3858,7 +4087,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1087</v>
       </c>
@@ -3880,14 +4109,17 @@
       <c r="I47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>540</v>
+      <c r="J47" s="6" t="s">
+        <v>530</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1067</v>
       </c>
@@ -3906,14 +4138,17 @@
       <c r="I48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>540</v>
+      <c r="J48" s="6" t="s">
+        <v>530</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1094</v>
       </c>
@@ -3933,7 +4168,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1093</v>
       </c>
@@ -3953,7 +4188,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1068</v>
       </c>
@@ -3970,7 +4205,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1682</v>
       </c>
@@ -3987,7 +4222,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1432</v>
       </c>
@@ -4004,7 +4239,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1239</v>
       </c>
@@ -4021,7 +4256,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1521</v>
       </c>
@@ -4041,7 +4276,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1221</v>
       </c>
@@ -4061,7 +4296,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1222</v>
       </c>
@@ -4084,13 +4319,16 @@
         <v>523</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>1223</v>
       </c>
@@ -4113,13 +4351,16 @@
         <v>524</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>1220</v>
       </c>
@@ -4136,16 +4377,19 @@
         <v>62</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1233</v>
       </c>
@@ -4165,7 +4409,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1234</v>
       </c>
@@ -4185,7 +4429,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1235</v>
       </c>
@@ -4205,7 +4449,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1236</v>
       </c>
@@ -4225,7 +4469,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>1232</v>
       </c>
@@ -4242,7 +4486,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>1429</v>
       </c>
@@ -4262,7 +4506,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>1431</v>
       </c>
@@ -4282,7 +4526,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>1430</v>
       </c>
@@ -4302,7 +4546,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>1238</v>
       </c>
@@ -4322,7 +4566,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>1237</v>
       </c>
@@ -4339,7 +4583,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>1611</v>
       </c>
@@ -4359,7 +4603,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>1230</v>
       </c>
@@ -4379,7 +4623,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1229</v>
       </c>
@@ -4396,7 +4640,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>1522</v>
       </c>
@@ -4415,8 +4659,21 @@
       <c r="H73" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>1225</v>
       </c>
@@ -4435,8 +4692,21 @@
       <c r="H74" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>1226</v>
       </c>
@@ -4455,8 +4725,21 @@
       <c r="H75" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>1610</v>
       </c>
@@ -4475,8 +4758,21 @@
       <c r="H76" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>1228</v>
       </c>
@@ -4495,8 +4791,12 @@
       <c r="H77" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>1428</v>
       </c>
@@ -4515,8 +4815,21 @@
       <c r="H78" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>1224</v>
       </c>
@@ -4532,8 +4845,21 @@
       <c r="H79" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="J79" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>1504</v>
       </c>
@@ -5299,10 +5625,10 @@
         <v>125</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -5328,13 +5654,13 @@
         <v>516</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
@@ -5357,13 +5683,13 @@
         <v>516</v>
       </c>
       <c r="I116" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
@@ -7281,7 +7607,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>1564</v>
       </c>
@@ -7298,7 +7624,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>1482</v>
       </c>
@@ -7315,7 +7641,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>1480</v>
       </c>
@@ -7343,8 +7669,14 @@
       <c r="J211" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L211" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M211" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>1481</v>
       </c>
@@ -7372,8 +7704,14 @@
       <c r="J212" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L212" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M212" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>1383</v>
       </c>
@@ -7398,8 +7736,14 @@
       <c r="J213" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L213" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M213" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>1561</v>
       </c>
@@ -7421,8 +7765,14 @@
       <c r="J214" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L214" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M214" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>1384</v>
       </c>
@@ -7442,13 +7792,19 @@
         <v>519</v>
       </c>
       <c r="I215" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="J215" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L215" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M215" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>1382</v>
       </c>
@@ -7468,13 +7824,19 @@
         <v>519</v>
       </c>
       <c r="I216" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J216" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L216" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M216" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>1381</v>
       </c>
@@ -7499,8 +7861,14 @@
       <c r="J217" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L217" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M217" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>1376</v>
       </c>
@@ -7528,8 +7896,14 @@
       <c r="J218" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L218" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M218" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>1379</v>
       </c>
@@ -7557,8 +7931,14 @@
       <c r="J219" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L219" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M219" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>1380</v>
       </c>
@@ -7586,8 +7966,14 @@
       <c r="J220" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L220" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M220" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>1377</v>
       </c>
@@ -7615,8 +8001,14 @@
       <c r="J221" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L221" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M221" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>1378</v>
       </c>
@@ -7644,8 +8036,14 @@
       <c r="J222" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L222" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M222" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>1372</v>
       </c>
@@ -7670,8 +8068,14 @@
       <c r="J223" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L223" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M223" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>1373</v>
       </c>
@@ -8002,7 +8406,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>1439</v>
       </c>
@@ -8025,10 +8429,16 @@
         <v>508</v>
       </c>
       <c r="J241" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+      <c r="L241" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M241" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>1567</v>
       </c>
@@ -8048,7 +8458,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>1568</v>
       </c>
@@ -8068,7 +8478,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>1569</v>
       </c>
@@ -8088,7 +8498,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>1570</v>
       </c>
@@ -8108,7 +8518,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>1571</v>
       </c>
@@ -8131,7 +8541,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>1573</v>
       </c>
@@ -8154,7 +8564,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>1674</v>
       </c>
@@ -8174,7 +8584,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>1313</v>
       </c>
@@ -8194,16 +8604,19 @@
         <v>519</v>
       </c>
       <c r="I249" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J249" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L249" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M249" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>1534</v>
       </c>
@@ -8226,13 +8639,16 @@
         <v>271</v>
       </c>
       <c r="J250" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L250" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M250" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>1533</v>
       </c>
@@ -8255,16 +8671,19 @@
         <v>519</v>
       </c>
       <c r="I251" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J251" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L251" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M251" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>1312</v>
       </c>
@@ -8287,16 +8706,19 @@
         <v>519</v>
       </c>
       <c r="I252" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J252" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L252" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M252" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>1532</v>
       </c>
@@ -8316,16 +8738,19 @@
         <v>519</v>
       </c>
       <c r="I253" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J253" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L253" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M253" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>1476</v>
       </c>
@@ -8345,16 +8770,19 @@
         <v>519</v>
       </c>
       <c r="I254" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J254" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L254" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M254" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>1535</v>
       </c>
@@ -8374,16 +8802,19 @@
         <v>519</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J255" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L255" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M255" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>1536</v>
       </c>
@@ -8403,16 +8834,19 @@
         <v>519</v>
       </c>
       <c r="I256" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J256" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L256" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M256" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>1311</v>
       </c>
@@ -8432,16 +8866,19 @@
         <v>519</v>
       </c>
       <c r="I257" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J257" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L257" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M257" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>1294</v>
       </c>
@@ -8458,16 +8895,19 @@
         <v>519</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J258" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L258" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M258" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>1308</v>
       </c>
@@ -8487,7 +8927,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>1617</v>
       </c>
@@ -8507,7 +8947,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>1309</v>
       </c>
@@ -8527,7 +8967,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>1310</v>
       </c>
@@ -8547,7 +8987,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>1293</v>
       </c>
@@ -8564,7 +9004,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>1407</v>
       </c>
@@ -8581,7 +9021,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>1629</v>
       </c>
@@ -8604,7 +9044,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>1627</v>
       </c>
@@ -8627,7 +9067,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>1630</v>
       </c>
@@ -8650,7 +9090,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>1628</v>
       </c>
@@ -8673,7 +9113,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>1626</v>
       </c>
@@ -8696,7 +9136,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>1655</v>
       </c>
@@ -8722,7 +9162,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>1656</v>
       </c>
@@ -8748,7 +9188,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>1654</v>
       </c>
@@ -9154,7 +9594,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>1633</v>
       </c>
@@ -9177,7 +9617,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>1644</v>
       </c>
@@ -9200,7 +9640,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>1645</v>
       </c>
@@ -9223,7 +9663,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>1646</v>
       </c>
@@ -9246,7 +9686,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>1538</v>
       </c>
@@ -9266,16 +9706,19 @@
         <v>519</v>
       </c>
       <c r="I293" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="J293" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="J293" s="1" t="s">
-        <v>531</v>
-      </c>
       <c r="L293" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M293" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>1466</v>
       </c>
@@ -9298,13 +9741,16 @@
         <v>320</v>
       </c>
       <c r="J294" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L294" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M294" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>1465</v>
       </c>
@@ -9324,16 +9770,19 @@
         <v>519</v>
       </c>
       <c r="I295" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J295" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L295" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M295" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>1537</v>
       </c>
@@ -9359,13 +9808,16 @@
         <v>323</v>
       </c>
       <c r="J296" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L296" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M296" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>1467</v>
       </c>
@@ -9385,10 +9837,13 @@
         <v>519</v>
       </c>
       <c r="L297" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M297" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>1477</v>
       </c>
@@ -9411,13 +9866,16 @@
         <v>324</v>
       </c>
       <c r="J298" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L298" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M298" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>1464</v>
       </c>
@@ -9440,13 +9898,16 @@
         <v>325</v>
       </c>
       <c r="J299" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L299" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M299" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>1295</v>
       </c>
@@ -9463,10 +9924,13 @@
         <v>519</v>
       </c>
       <c r="L300" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M300" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>1541</v>
       </c>
@@ -9485,14 +9949,11 @@
       <c r="H301" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="I301" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="J301" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N301" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>1544</v>
       </c>
@@ -9511,14 +9972,11 @@
       <c r="H302" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="I302" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="J302" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N302" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>1542</v>
       </c>
@@ -9541,10 +9999,16 @@
         <v>329</v>
       </c>
       <c r="J303" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+      <c r="L303" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="M303" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>1406</v>
       </c>
@@ -10228,7 +10692,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <v>1263</v>
       </c>
@@ -10251,16 +10715,16 @@
         <v>519</v>
       </c>
       <c r="I337" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J337" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K337" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <v>1259</v>
       </c>
@@ -10283,16 +10747,16 @@
         <v>519</v>
       </c>
       <c r="I338" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J338" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K338" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <v>1261</v>
       </c>
@@ -10315,16 +10779,16 @@
         <v>519</v>
       </c>
       <c r="I339" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K339" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>1260</v>
       </c>
@@ -10347,16 +10811,16 @@
         <v>519</v>
       </c>
       <c r="I340" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J340" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K340" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <v>1397</v>
       </c>
@@ -10379,16 +10843,16 @@
         <v>519</v>
       </c>
       <c r="I341" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J341" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K341" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <v>1262</v>
       </c>
@@ -10411,16 +10875,16 @@
         <v>519</v>
       </c>
       <c r="I342" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="J342" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="K342" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <v>1258</v>
       </c>
@@ -10440,13 +10904,13 @@
         <v>519</v>
       </c>
       <c r="I343" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J343" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <v>1250</v>
       </c>
@@ -10469,13 +10933,13 @@
         <v>519</v>
       </c>
       <c r="I344" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J344" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <v>1523</v>
       </c>
@@ -10498,13 +10962,13 @@
         <v>519</v>
       </c>
       <c r="I345" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J345" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <v>1249</v>
       </c>
@@ -10524,13 +10988,13 @@
         <v>519</v>
       </c>
       <c r="I346" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J346" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <v>1264</v>
       </c>
@@ -10553,13 +11017,16 @@
         <v>374</v>
       </c>
       <c r="J347" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="L347" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M347" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <v>1245</v>
       </c>
@@ -10582,7 +11049,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <v>1246</v>
       </c>
@@ -10605,7 +11072,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <v>1247</v>
       </c>
@@ -10628,7 +11095,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <v>1248</v>
       </c>
@@ -10651,7 +11118,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <v>1244</v>
       </c>
@@ -10671,7 +11138,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A353" s="2">
         <v>1265</v>
       </c>
@@ -10694,13 +11161,16 @@
         <v>380</v>
       </c>
       <c r="J353" s="1" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
       <c r="L353" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M353" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <v>1525</v>
       </c>
@@ -10723,7 +11193,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <v>1683</v>
       </c>
@@ -10746,7 +11216,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <v>1436</v>
       </c>
@@ -10769,7 +11239,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <v>1659</v>
       </c>
@@ -10792,7 +11262,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <v>1437</v>
       </c>
@@ -10815,7 +11285,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <v>1526</v>
       </c>
@@ -10838,7 +11308,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>1434</v>
       </c>
@@ -10858,7 +11328,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>1256</v>
       </c>
@@ -10881,7 +11351,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>1468</v>
       </c>
@@ -10904,7 +11374,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <v>1255</v>
       </c>
@@ -10927,7 +11397,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <v>1257</v>
       </c>
@@ -10950,7 +11420,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <v>1254</v>
       </c>
@@ -10970,7 +11440,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <v>1252</v>
       </c>
@@ -10993,7 +11463,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <v>1524</v>
       </c>
@@ -11016,7 +11486,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <v>1251</v>
       </c>
@@ -11036,7 +11506,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A369" s="2">
         <v>1470</v>
       </c>
@@ -11055,11 +11525,20 @@
       <c r="H369" s="1" t="s">
         <v>519</v>
       </c>
+      <c r="I369" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="J369" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="L369" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M369" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A370" s="2">
         <v>1287</v>
       </c>
@@ -11079,16 +11558,19 @@
         <v>519</v>
       </c>
       <c r="I370" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J370" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L370" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M370" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371" s="2">
         <v>1290</v>
       </c>
@@ -11108,19 +11590,16 @@
         <v>519</v>
       </c>
       <c r="I371" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J371" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="K371" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="L371" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372" s="2">
         <v>1531</v>
       </c>
@@ -11143,7 +11622,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373" s="2">
         <v>1286</v>
       </c>
@@ -11163,16 +11642,19 @@
         <v>519</v>
       </c>
       <c r="I373" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="J373" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="J373" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="L373" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M373" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A374" s="2">
         <v>1616</v>
       </c>
@@ -11191,11 +11673,20 @@
       <c r="H374" s="1" t="s">
         <v>519</v>
       </c>
+      <c r="I374" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="J374" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="L374" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M374" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375" s="2">
         <v>1291</v>
       </c>
@@ -11215,16 +11706,19 @@
         <v>519</v>
       </c>
       <c r="I375" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="J375" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="J375" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="L375" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M375" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A376" s="2">
         <v>1288</v>
       </c>
@@ -11247,13 +11741,16 @@
         <v>403</v>
       </c>
       <c r="J376" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L376" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M376" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <v>1615</v>
       </c>
@@ -11273,16 +11770,19 @@
         <v>519</v>
       </c>
       <c r="I377" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J377" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L377" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M377" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378" s="2">
         <v>1469</v>
       </c>
@@ -11302,16 +11802,19 @@
         <v>519</v>
       </c>
       <c r="I378" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J378" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L378" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M378" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A379" s="2">
         <v>1289</v>
       </c>
@@ -11334,16 +11837,13 @@
         <v>406</v>
       </c>
       <c r="J379" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="K379" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="L379" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A380" s="2">
         <v>1614</v>
       </c>
@@ -11366,13 +11866,16 @@
         <v>407</v>
       </c>
       <c r="J380" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L380" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M380" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <v>1408</v>
       </c>
@@ -11395,16 +11898,19 @@
         <v>519</v>
       </c>
       <c r="I381" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J381" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L381" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M381" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <v>1409</v>
       </c>
@@ -11427,16 +11933,19 @@
         <v>519</v>
       </c>
       <c r="I382" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J382" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L382" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M382" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <v>1410</v>
       </c>
@@ -11459,16 +11968,19 @@
         <v>519</v>
       </c>
       <c r="I383" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J383" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="L383" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M383" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A384" s="2">
         <v>1243</v>
       </c>
@@ -11484,8 +11996,17 @@
       <c r="H384" s="1" t="s">
         <v>519</v>
       </c>
+      <c r="I384" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="J384" s="1" t="s">
+        <v>545</v>
+      </c>
       <c r="L384" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
+      </c>
+      <c r="M384" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="385" spans="1:8" x14ac:dyDescent="0.25">
@@ -11817,7 +12338,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="401" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A401" s="2">
         <v>1210</v>
       </c>
@@ -11837,7 +12358,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="402" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A402" s="2">
         <v>1214</v>
       </c>
@@ -11857,7 +12378,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="403" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A403" s="2">
         <v>1679</v>
       </c>
@@ -11877,7 +12398,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="404" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A404" s="2">
         <v>1194</v>
       </c>
@@ -11900,13 +12421,13 @@
         <v>434</v>
       </c>
       <c r="J404" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K404" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="405" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A405" s="2">
         <v>1193</v>
       </c>
@@ -11929,13 +12450,13 @@
         <v>435</v>
       </c>
       <c r="J405" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K405" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="406" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A406" s="2">
         <v>1192</v>
       </c>
@@ -11952,16 +12473,16 @@
         <v>493</v>
       </c>
       <c r="I406" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J406" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="K406" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="407" spans="1:12" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A407" s="2">
         <v>1200</v>
       </c>
@@ -11978,7 +12499,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="408" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A408" s="2">
         <v>1514</v>
       </c>
@@ -11998,7 +12519,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="409" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A409" s="2">
         <v>1515</v>
       </c>
@@ -12018,7 +12539,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="410" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A410" s="2">
         <v>1196</v>
       </c>
@@ -12035,7 +12556,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="411" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A411" s="2">
         <v>1111</v>
       </c>
@@ -12058,10 +12579,13 @@
         <v>525</v>
       </c>
       <c r="L411" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="412" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M411" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="412" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A412" s="2">
         <v>1114</v>
       </c>
@@ -12078,16 +12602,19 @@
         <v>519</v>
       </c>
       <c r="I412" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J412" s="1" t="s">
         <v>525</v>
       </c>
       <c r="L412" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="413" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M412" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A413" s="2">
         <v>1112</v>
       </c>
@@ -12110,10 +12637,13 @@
         <v>525</v>
       </c>
       <c r="L413" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="414" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M413" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A414" s="2">
         <v>1496</v>
       </c>
@@ -12133,16 +12663,19 @@
         <v>519</v>
       </c>
       <c r="I414" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J414" s="1" t="s">
         <v>525</v>
       </c>
       <c r="L414" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="415" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M414" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A415" s="2">
         <v>1412</v>
       </c>
@@ -12162,16 +12695,19 @@
         <v>519</v>
       </c>
       <c r="I415" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J415" s="1" t="s">
         <v>525</v>
       </c>
       <c r="L415" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="416" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M415" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A416" s="2">
         <v>1472</v>
       </c>
@@ -12197,10 +12733,13 @@
         <v>525</v>
       </c>
       <c r="L416" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M416" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A417" s="2">
         <v>1113</v>
       </c>
@@ -12217,16 +12756,19 @@
         <v>519</v>
       </c>
       <c r="I417" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J417" s="1" t="s">
         <v>525</v>
       </c>
       <c r="L417" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="M417" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A418" s="2">
         <v>1499</v>
       </c>
@@ -12249,7 +12791,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="419" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A419" s="2">
         <v>1421</v>
       </c>
@@ -12272,7 +12814,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="420" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A420" s="2">
         <v>1420</v>
       </c>
@@ -12295,7 +12837,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="421" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A421" s="2">
         <v>1597</v>
       </c>
@@ -12318,7 +12860,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="422" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A422" s="2">
         <v>1500</v>
       </c>
@@ -12341,7 +12883,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="423" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A423" s="2">
         <v>1415</v>
       </c>
@@ -12361,7 +12903,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="424" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A424" s="2">
         <v>1416</v>
       </c>
@@ -12384,7 +12926,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="425" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A425" s="2">
         <v>1417</v>
       </c>
@@ -12407,7 +12949,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="426" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A426" s="2">
         <v>1413</v>
       </c>
@@ -12427,7 +12969,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="427" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A427" s="2">
         <v>1418</v>
       </c>
@@ -12450,7 +12992,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A428" s="2">
         <v>1598</v>
       </c>
@@ -12473,7 +13015,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A429" s="2">
         <v>1419</v>
       </c>
@@ -12496,7 +13038,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A430" s="2">
         <v>1414</v>
       </c>
@@ -12516,7 +13058,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A431" s="2">
         <v>1120</v>
       </c>
@@ -12536,7 +13078,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="432" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A432" s="2">
         <v>1122</v>
       </c>

</xml_diff>

<commit_message>
Implemented adjustments to hypertension dataset and Neo's tables as per meeting on 12/03/20
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2822" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="582">
   <si>
     <t>coding</t>
   </si>
@@ -1701,12 +1701,6 @@
     <t>ComorbidityGroup</t>
   </si>
   <si>
-    <t>Group C</t>
-  </si>
-  <si>
-    <t>Group B</t>
-  </si>
-  <si>
     <t>(blank, no longer categorized as stroke) - no longer in the grouping because technically not a chronic condition</t>
   </si>
   <si>
@@ -1759,13 +1753,28 @@
   </si>
   <si>
     <t>Communicable Disease</t>
+  </si>
+  <si>
+    <t>Asthma or COPD</t>
+  </si>
+  <si>
+    <t>Migraine</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Back pain</t>
+  </si>
+  <si>
+    <t>Other chronic comorbidities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1899,6 +1908,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -2296,11 +2311,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2653,11 +2668,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N447"/>
+  <dimension ref="A1:Q447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L377" sqref="L377"/>
+      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,10 +2728,10 @@
         <v>558</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2768,7 +2783,7 @@
         <v>538</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>538</v>
@@ -2803,7 +2818,7 @@
         <v>538</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>538</v>
@@ -2838,7 +2853,7 @@
         <v>538</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>538</v>
@@ -2870,7 +2885,7 @@
         <v>538</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>538</v>
@@ -2896,7 +2911,7 @@
         <v>519</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2925,7 +2940,7 @@
         <v>538</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>538</v>
@@ -2957,7 +2972,7 @@
         <v>538</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>538</v>
@@ -2991,14 +3006,14 @@
       <c r="J10" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L10" s="7" t="s">
-        <v>559</v>
+      <c r="L10" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3026,11 +3041,11 @@
       <c r="J11" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>559</v>
+      <c r="L11" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3062,10 +3077,10 @@
         <v>530</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3097,10 +3112,10 @@
         <v>530</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3271,7 +3286,7 @@
         <v>538</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>538</v>
@@ -3337,11 +3352,11 @@
       <c r="J21" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>559</v>
+      <c r="L21" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -3375,11 +3390,11 @@
       <c r="J22" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L22" s="6" t="s">
-        <v>559</v>
+      <c r="L22" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -3410,11 +3425,11 @@
       <c r="J23" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L23" s="6" t="s">
-        <v>559</v>
+      <c r="L23" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3448,11 +3463,11 @@
       <c r="J24" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>559</v>
+      <c r="L24" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3486,11 +3501,11 @@
       <c r="J25" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>559</v>
+      <c r="L25" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -3524,11 +3539,11 @@
       <c r="J26" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L26" s="6" t="s">
-        <v>559</v>
+      <c r="L26" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3559,11 +3574,11 @@
       <c r="J27" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L27" s="6" t="s">
-        <v>559</v>
+      <c r="L27" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -3591,11 +3606,11 @@
       <c r="J28" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>559</v>
+      <c r="L28" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -3623,11 +3638,11 @@
       <c r="J29" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L29" s="6" t="s">
-        <v>559</v>
+      <c r="L29" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3658,11 +3673,11 @@
       <c r="J30" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>559</v>
+      <c r="L30" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3693,11 +3708,11 @@
       <c r="J31" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L31" s="6" t="s">
-        <v>559</v>
+      <c r="L31" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3725,11 +3740,11 @@
       <c r="J32" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L32" s="6" t="s">
-        <v>559</v>
+      <c r="L32" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3780,11 +3795,11 @@
       <c r="J34" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>559</v>
+      <c r="L34" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3809,11 +3824,11 @@
       <c r="J35" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L35" s="6" t="s">
-        <v>559</v>
+      <c r="L35" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3898,11 +3913,11 @@
       <c r="J39" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>559</v>
+      <c r="L39" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3991,11 +4006,11 @@
         <v>530</v>
       </c>
       <c r="K43" s="6"/>
-      <c r="L43" s="6" t="s">
-        <v>559</v>
+      <c r="L43" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -4027,11 +4042,11 @@
         <v>530</v>
       </c>
       <c r="K44" s="6"/>
-      <c r="L44" s="6" t="s">
-        <v>559</v>
+      <c r="L44" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -4060,11 +4075,11 @@
         <v>530</v>
       </c>
       <c r="K45" s="6"/>
-      <c r="L45" s="6" t="s">
-        <v>559</v>
+      <c r="L45" s="1" t="s">
+        <v>538</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -4113,10 +4128,10 @@
         <v>530</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -4142,10 +4157,10 @@
         <v>530</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -4322,10 +4337,10 @@
         <v>533</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -4354,10 +4369,10 @@
         <v>533</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -4383,10 +4398,10 @@
         <v>533</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -4663,14 +4678,14 @@
         <v>81</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K73" s="6"/>
-      <c r="L73" s="6" t="s">
-        <v>559</v>
+      <c r="L73" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4693,17 +4708,17 @@
         <v>519</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K74" s="6"/>
-      <c r="L74" s="6" t="s">
-        <v>559</v>
+      <c r="L74" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4726,17 +4741,17 @@
         <v>519</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K75" s="6"/>
-      <c r="L75" s="6" t="s">
-        <v>559</v>
+      <c r="L75" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4759,17 +4774,17 @@
         <v>519</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K76" s="6"/>
-      <c r="L76" s="6" t="s">
-        <v>559</v>
+      <c r="L76" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4819,14 +4834,14 @@
         <v>86</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K78" s="6"/>
-      <c r="L78" s="6" t="s">
-        <v>559</v>
+      <c r="L78" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4846,17 +4861,17 @@
         <v>519</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="K79" s="6"/>
-      <c r="L79" s="6" t="s">
-        <v>559</v>
+      <c r="L79" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -7669,11 +7684,11 @@
       <c r="J211" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L211" s="6" t="s">
-        <v>559</v>
+      <c r="L211" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M211" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -7704,11 +7719,11 @@
       <c r="J212" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L212" s="6" t="s">
-        <v>559</v>
+      <c r="L212" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M212" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -7736,11 +7751,11 @@
       <c r="J213" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L213" s="6" t="s">
-        <v>559</v>
+      <c r="L213" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M213" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
@@ -7765,11 +7780,11 @@
       <c r="J214" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L214" s="6" t="s">
-        <v>559</v>
+      <c r="L214" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M214" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -7797,11 +7812,11 @@
       <c r="J215" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L215" s="6" t="s">
-        <v>559</v>
+      <c r="L215" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M215" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
@@ -7829,11 +7844,11 @@
       <c r="J216" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L216" s="6" t="s">
-        <v>559</v>
+      <c r="L216" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M216" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
@@ -7861,11 +7876,11 @@
       <c r="J217" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L217" s="6" t="s">
-        <v>559</v>
+      <c r="L217" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M217" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
@@ -7896,11 +7911,11 @@
       <c r="J218" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L218" s="6" t="s">
-        <v>559</v>
+      <c r="L218" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M218" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
@@ -7931,11 +7946,11 @@
       <c r="J219" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L219" s="6" t="s">
-        <v>559</v>
+      <c r="L219" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M219" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
@@ -7966,11 +7981,11 @@
       <c r="J220" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L220" s="6" t="s">
-        <v>559</v>
+      <c r="L220" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M220" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
@@ -8001,11 +8016,11 @@
       <c r="J221" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L221" s="6" t="s">
-        <v>559</v>
+      <c r="L221" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M221" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
@@ -8036,11 +8051,11 @@
       <c r="J222" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L222" s="6" t="s">
-        <v>559</v>
+      <c r="L222" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M222" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.25">
@@ -8068,11 +8083,11 @@
       <c r="J223" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L223" s="6" t="s">
-        <v>559</v>
+      <c r="L223" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M223" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.25">
@@ -8431,11 +8446,11 @@
       <c r="J241" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="L241" s="6" t="s">
-        <v>559</v>
+      <c r="L241" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M241" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.25">
@@ -8610,10 +8625,10 @@
         <v>529</v>
       </c>
       <c r="L249" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M249" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
@@ -8642,10 +8657,10 @@
         <v>529</v>
       </c>
       <c r="L250" s="1" t="s">
-        <v>559</v>
+        <v>580</v>
       </c>
       <c r="M250" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
@@ -8677,10 +8692,10 @@
         <v>529</v>
       </c>
       <c r="L251" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M251" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.25">
@@ -8712,10 +8727,10 @@
         <v>529</v>
       </c>
       <c r="L252" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M252" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
@@ -8744,10 +8759,10 @@
         <v>529</v>
       </c>
       <c r="L253" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M253" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.25">
@@ -8776,10 +8791,10 @@
         <v>529</v>
       </c>
       <c r="L254" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M254" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.25">
@@ -8808,10 +8823,10 @@
         <v>529</v>
       </c>
       <c r="L255" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M255" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.25">
@@ -8840,10 +8855,10 @@
         <v>529</v>
       </c>
       <c r="L256" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M256" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -8872,10 +8887,10 @@
         <v>529</v>
       </c>
       <c r="L257" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M257" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.25">
@@ -8901,10 +8916,10 @@
         <v>529</v>
       </c>
       <c r="L258" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M258" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.25">
@@ -9712,10 +9727,10 @@
         <v>529</v>
       </c>
       <c r="L293" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M293" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="294" spans="1:14" x14ac:dyDescent="0.25">
@@ -9744,10 +9759,10 @@
         <v>529</v>
       </c>
       <c r="L294" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M294" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="295" spans="1:14" x14ac:dyDescent="0.25">
@@ -9776,10 +9791,10 @@
         <v>529</v>
       </c>
       <c r="L295" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M295" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="296" spans="1:14" x14ac:dyDescent="0.25">
@@ -9811,10 +9826,10 @@
         <v>529</v>
       </c>
       <c r="L296" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M296" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="297" spans="1:14" x14ac:dyDescent="0.25">
@@ -9837,10 +9852,10 @@
         <v>519</v>
       </c>
       <c r="L297" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M297" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="298" spans="1:14" x14ac:dyDescent="0.25">
@@ -9869,10 +9884,10 @@
         <v>529</v>
       </c>
       <c r="L298" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M298" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="299" spans="1:14" x14ac:dyDescent="0.25">
@@ -9901,10 +9916,10 @@
         <v>529</v>
       </c>
       <c r="L299" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M299" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="300" spans="1:14" x14ac:dyDescent="0.25">
@@ -9924,10 +9939,10 @@
         <v>519</v>
       </c>
       <c r="L300" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M300" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="301" spans="1:14" x14ac:dyDescent="0.25">
@@ -9950,7 +9965,7 @@
         <v>519</v>
       </c>
       <c r="N301" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="302" spans="1:14" x14ac:dyDescent="0.25">
@@ -9973,7 +9988,7 @@
         <v>519</v>
       </c>
       <c r="N302" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="303" spans="1:14" x14ac:dyDescent="0.25">
@@ -10001,11 +10016,11 @@
       <c r="J303" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L303" s="6" t="s">
-        <v>559</v>
+      <c r="L303" s="1" t="s">
+        <v>581</v>
       </c>
       <c r="M303" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="304" spans="1:14" x14ac:dyDescent="0.25">
@@ -10718,7 +10733,7 @@
         <v>548</v>
       </c>
       <c r="J337" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K337" s="1" t="s">
         <v>557</v>
@@ -10750,7 +10765,7 @@
         <v>549</v>
       </c>
       <c r="J338" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K338" s="1" t="s">
         <v>557</v>
@@ -10782,7 +10797,7 @@
         <v>549</v>
       </c>
       <c r="J339" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K339" s="1" t="s">
         <v>557</v>
@@ -10814,7 +10829,7 @@
         <v>549</v>
       </c>
       <c r="J340" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K340" s="1" t="s">
         <v>557</v>
@@ -10846,7 +10861,7 @@
         <v>549</v>
       </c>
       <c r="J341" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K341" s="1" t="s">
         <v>557</v>
@@ -10878,7 +10893,7 @@
         <v>547</v>
       </c>
       <c r="J342" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K342" s="1" t="s">
         <v>557</v>
@@ -10907,7 +10922,7 @@
         <v>549</v>
       </c>
       <c r="J343" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
@@ -10936,7 +10951,7 @@
         <v>549</v>
       </c>
       <c r="J344" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
@@ -10965,7 +10980,7 @@
         <v>549</v>
       </c>
       <c r="J345" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.25">
@@ -10991,7 +11006,7 @@
         <v>549</v>
       </c>
       <c r="J346" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
@@ -11017,13 +11032,13 @@
         <v>374</v>
       </c>
       <c r="J347" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L347" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M347" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.25">
@@ -11138,7 +11153,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A353" s="2">
         <v>1265</v>
       </c>
@@ -11161,16 +11176,18 @@
         <v>380</v>
       </c>
       <c r="J353" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L353" s="1" t="s">
-        <v>559</v>
+        <v>578</v>
       </c>
       <c r="M353" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="P353" s="8"/>
+      <c r="Q353" s="8"/>
+    </row>
+    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <v>1525</v>
       </c>
@@ -11192,8 +11209,10 @@
       <c r="H354" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P354" s="8"/>
+      <c r="Q354" s="8"/>
+    </row>
+    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <v>1683</v>
       </c>
@@ -11215,8 +11234,10 @@
       <c r="H355" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P355" s="8"/>
+      <c r="Q355" s="8"/>
+    </row>
+    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <v>1436</v>
       </c>
@@ -11238,8 +11259,10 @@
       <c r="H356" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P356" s="8"/>
+      <c r="Q356" s="8"/>
+    </row>
+    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <v>1659</v>
       </c>
@@ -11261,8 +11284,10 @@
       <c r="H357" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P357" s="8"/>
+      <c r="Q357" s="8"/>
+    </row>
+    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <v>1437</v>
       </c>
@@ -11284,8 +11309,10 @@
       <c r="H358" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P358" s="8"/>
+      <c r="Q358" s="8"/>
+    </row>
+    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <v>1526</v>
       </c>
@@ -11307,8 +11334,10 @@
       <c r="H359" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P359" s="8"/>
+      <c r="Q359" s="8"/>
+    </row>
+    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>1434</v>
       </c>
@@ -11327,8 +11356,9 @@
       <c r="H360" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P360" s="8"/>
+    </row>
+    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>1256</v>
       </c>
@@ -11350,8 +11380,9 @@
       <c r="H361" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P361" s="8"/>
+    </row>
+    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>1468</v>
       </c>
@@ -11373,8 +11404,9 @@
       <c r="H362" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P362" s="8"/>
+    </row>
+    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <v>1255</v>
       </c>
@@ -11397,7 +11429,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <v>1257</v>
       </c>
@@ -11420,7 +11452,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <v>1254</v>
       </c>
@@ -11440,7 +11472,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <v>1252</v>
       </c>
@@ -11463,7 +11495,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <v>1524</v>
       </c>
@@ -11486,7 +11518,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <v>1251</v>
       </c>
@@ -11526,13 +11558,13 @@
         <v>519</v>
       </c>
       <c r="I369" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="J369" s="1" t="s">
         <v>545</v>
       </c>
       <c r="L369" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M369" s="1" t="s">
         <v>545</v>
@@ -11564,7 +11596,7 @@
         <v>545</v>
       </c>
       <c r="L370" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M370" s="1" t="s">
         <v>545</v>
@@ -11648,7 +11680,7 @@
         <v>545</v>
       </c>
       <c r="L373" s="1" t="s">
-        <v>559</v>
+        <v>579</v>
       </c>
       <c r="M373" s="1" t="s">
         <v>545</v>
@@ -11673,14 +11705,14 @@
       <c r="H374" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="I374" s="8" t="s">
+      <c r="I374" s="7" t="s">
         <v>401</v>
       </c>
       <c r="J374" s="1" t="s">
         <v>545</v>
       </c>
       <c r="L374" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M374" s="1" t="s">
         <v>545</v>
@@ -11712,7 +11744,7 @@
         <v>545</v>
       </c>
       <c r="L375" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M375" s="1" t="s">
         <v>545</v>
@@ -11744,7 +11776,7 @@
         <v>545</v>
       </c>
       <c r="L376" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M376" s="1" t="s">
         <v>545</v>
@@ -11776,7 +11808,7 @@
         <v>545</v>
       </c>
       <c r="L377" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M377" s="1" t="s">
         <v>545</v>
@@ -11808,7 +11840,7 @@
         <v>545</v>
       </c>
       <c r="L378" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M378" s="1" t="s">
         <v>545</v>
@@ -11869,7 +11901,7 @@
         <v>545</v>
       </c>
       <c r="L380" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M380" s="1" t="s">
         <v>545</v>
@@ -11904,7 +11936,7 @@
         <v>545</v>
       </c>
       <c r="L381" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M381" s="1" t="s">
         <v>545</v>
@@ -11939,7 +11971,7 @@
         <v>545</v>
       </c>
       <c r="L382" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M382" s="1" t="s">
         <v>545</v>
@@ -11974,7 +12006,7 @@
         <v>545</v>
       </c>
       <c r="L383" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M383" s="1" t="s">
         <v>545</v>
@@ -11997,19 +12029,19 @@
         <v>519</v>
       </c>
       <c r="I384" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="J384" s="1" t="s">
         <v>545</v>
       </c>
       <c r="L384" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M384" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="2">
         <v>1202</v>
       </c>
@@ -12029,7 +12061,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="2">
         <v>1201</v>
       </c>
@@ -12046,7 +12078,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="2">
         <v>1197</v>
       </c>
@@ -12063,7 +12095,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="2">
         <v>1607</v>
       </c>
@@ -12085,8 +12117,11 @@
       <c r="H388" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K388" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="2">
         <v>1520</v>
       </c>
@@ -12108,8 +12143,11 @@
       <c r="H389" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K389" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="2">
         <v>1519</v>
       </c>
@@ -12128,8 +12166,11 @@
       <c r="H390" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K390" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="2">
         <v>1609</v>
       </c>
@@ -12151,8 +12192,11 @@
       <c r="H391" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K391" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="2">
         <v>1608</v>
       </c>
@@ -12171,8 +12215,11 @@
       <c r="H392" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K392" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="2">
         <v>1427</v>
       </c>
@@ -12191,8 +12238,11 @@
       <c r="H393" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K393" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="2">
         <v>1405</v>
       </c>
@@ -12208,8 +12258,11 @@
       <c r="H394" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K394" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="2">
         <v>1518</v>
       </c>
@@ -12229,7 +12282,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="2">
         <v>1404</v>
       </c>
@@ -12249,7 +12302,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="2">
         <v>1516</v>
       </c>
@@ -12272,7 +12325,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="2">
         <v>1396</v>
       </c>
@@ -12295,7 +12348,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="2">
         <v>1517</v>
       </c>
@@ -12318,7 +12371,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="2">
         <v>1207</v>
       </c>
@@ -12579,10 +12632,10 @@
         <v>525</v>
       </c>
       <c r="L411" s="1" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
       <c r="M411" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="412" spans="1:13" x14ac:dyDescent="0.25">
@@ -12608,10 +12661,10 @@
         <v>525</v>
       </c>
       <c r="L412" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M412" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="413" spans="1:13" x14ac:dyDescent="0.25">
@@ -12637,10 +12690,10 @@
         <v>525</v>
       </c>
       <c r="L413" s="1" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
       <c r="M413" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="414" spans="1:13" x14ac:dyDescent="0.25">
@@ -12669,10 +12722,10 @@
         <v>525</v>
       </c>
       <c r="L414" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M414" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="415" spans="1:13" x14ac:dyDescent="0.25">
@@ -12701,10 +12754,10 @@
         <v>525</v>
       </c>
       <c r="L415" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M415" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="416" spans="1:13" x14ac:dyDescent="0.25">
@@ -12733,10 +12786,10 @@
         <v>525</v>
       </c>
       <c r="L416" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M416" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.25">
@@ -12762,10 +12815,10 @@
         <v>525</v>
       </c>
       <c r="L417" s="1" t="s">
-        <v>559</v>
+        <v>581</v>
       </c>
       <c r="M417" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="418" spans="1:13" x14ac:dyDescent="0.25">
@@ -13387,7 +13440,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <protectedRanges>
     <protectedRange sqref="A1:XFD1" name="AllowFilter"/>
   </protectedRanges>

</xml_diff>

<commit_message>
Revised heart and kidney failure - removed from exclusions, added to comorbidities of interest
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="583">
   <si>
     <t>coding</t>
   </si>
@@ -1768,6 +1768,9 @@
   </si>
   <si>
     <t>Other chronic comorbidities</t>
+  </si>
+  <si>
+    <t>Kidney Failure</t>
   </si>
 </sst>
 </file>
@@ -2671,8 +2674,8 @@
   <dimension ref="A1:Q447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <pane ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M405" sqref="M405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,8 +3320,11 @@
       <c r="J20" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>557</v>
+      <c r="L20" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -12476,8 +12482,11 @@
       <c r="J404" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="K404" s="1" t="s">
-        <v>557</v>
+      <c r="L404" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="M404" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="405" spans="1:13" x14ac:dyDescent="0.25">
@@ -12531,8 +12540,11 @@
       <c r="J406" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="K406" s="1" t="s">
-        <v>557</v>
+      <c r="L406" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="M406" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="407" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Began implementing changes requested by Neo on ManuscriptResults_Feedback20200416 - changed comorbidities, re-ordered some covariates in tables, added header rows to reduce manual work on tables
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -15,14 +15,14 @@
     <sheet name="NonCancerIllness" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NonCancerIllness!$A$1:$L$447</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NonCancerIllness!$A$1:$Q$447</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="583">
   <si>
     <t>coding</t>
   </si>
@@ -1737,9 +1737,6 @@
     <t>Other cardiac</t>
   </si>
   <si>
-    <t>Musculoskeletal - chronic pain</t>
-  </si>
-  <si>
     <t>Chronic Respiratory Disease</t>
   </si>
   <si>
@@ -1749,12 +1746,6 @@
     <t>NB. including cardiomyopathy as one of the comorbidity diagnoses in Group C</t>
   </si>
   <si>
-    <t>Connective Tissue Disorder</t>
-  </si>
-  <si>
-    <t>Communicable Disease</t>
-  </si>
-  <si>
     <t>Asthma or COPD</t>
   </si>
   <si>
@@ -1764,13 +1755,22 @@
     <t>Depression</t>
   </si>
   <si>
-    <t>Back pain</t>
-  </si>
-  <si>
-    <t>Other chronic comorbidities</t>
-  </si>
-  <si>
-    <t>Kidney Failure</t>
+    <t>UKBTapela_HTN_ManuscriptResults_Feedback20200416.docx "Please remove back pain (do not fold into 'other chronic conditions')</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>20201604 "Is it possible to have anxiety and depression as two separate comorbidity diagnoses"</t>
+  </si>
+  <si>
+    <t>Arrhythmia</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Heart disease</t>
   </si>
 </sst>
 </file>
@@ -2670,12 +2670,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:Q447"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M405" sqref="M405"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,10 +2686,10 @@
     <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="17" style="1" customWidth="1"/>
+    <col min="9" max="10" width="17" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2734,10 +2734,10 @@
         <v>569</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1425</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>538</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>538</v>
@@ -2821,7 +2821,7 @@
         <v>538</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>538</v>
@@ -2856,7 +2856,7 @@
         <v>538</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>538</v>
@@ -2888,13 +2888,13 @@
         <v>538</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1083</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>538</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>538</v>
+        <v>581</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>538</v>
@@ -2975,13 +2975,13 @@
         <v>538</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1588</v>
       </c>
@@ -3009,17 +3009,11 @@
       <c r="J10" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>570</v>
-      </c>
       <c r="N10" s="1" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1079</v>
       </c>
@@ -3043,12 +3037,6 @@
       </c>
       <c r="J11" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3080,7 +3068,7 @@
         <v>530</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>570</v>
@@ -3115,13 +3103,13 @@
         <v>530</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1485</v>
       </c>
@@ -3150,7 +3138,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1486</v>
       </c>
@@ -3179,7 +3167,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1487</v>
       </c>
@@ -3208,7 +3196,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1484</v>
       </c>
@@ -3237,7 +3225,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1077</v>
       </c>
@@ -3289,13 +3277,13 @@
         <v>538</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1076</v>
       </c>
@@ -3320,14 +3308,11 @@
       <c r="J20" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1587</v>
       </c>
@@ -3358,14 +3343,8 @@
       <c r="J21" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1490</v>
       </c>
@@ -3396,14 +3375,8 @@
       <c r="J22" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1586</v>
       </c>
@@ -3431,14 +3404,8 @@
       <c r="J23" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1585</v>
       </c>
@@ -3469,14 +3436,8 @@
       <c r="J24" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1489</v>
       </c>
@@ -3507,14 +3468,8 @@
       <c r="J25" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1488</v>
       </c>
@@ -3545,14 +3500,8 @@
       <c r="J26" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1584</v>
       </c>
@@ -3580,14 +3529,8 @@
       <c r="J27" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1078</v>
       </c>
@@ -3612,14 +3555,8 @@
       <c r="J28" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1426</v>
       </c>
@@ -3644,14 +3581,8 @@
       <c r="J29" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1590</v>
       </c>
@@ -3679,14 +3610,8 @@
       <c r="J30" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1589</v>
       </c>
@@ -3714,14 +3639,8 @@
       <c r="J31" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1080</v>
       </c>
@@ -3746,14 +3665,8 @@
       <c r="J32" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1479</v>
       </c>
@@ -3779,7 +3692,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1066</v>
       </c>
@@ -3801,14 +3714,8 @@
       <c r="J34" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1473</v>
       </c>
@@ -3830,14 +3737,8 @@
       <c r="J35" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1072</v>
       </c>
@@ -3857,7 +3758,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1073</v>
       </c>
@@ -3877,7 +3778,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1065</v>
       </c>
@@ -3894,7 +3795,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1495</v>
       </c>
@@ -3919,14 +3820,8 @@
       <c r="J39" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1593</v>
       </c>
@@ -3946,7 +3841,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1494</v>
       </c>
@@ -3966,7 +3861,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1493</v>
       </c>
@@ -4013,7 +3908,7 @@
       </c>
       <c r="K43" s="6"/>
       <c r="L43" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>570</v>
@@ -4049,7 +3944,7 @@
       </c>
       <c r="K44" s="6"/>
       <c r="L44" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>570</v>
@@ -4082,13 +3977,13 @@
       </c>
       <c r="K45" s="6"/>
       <c r="L45" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1088</v>
       </c>
@@ -4134,7 +4029,7 @@
         <v>530</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>570</v>
@@ -4163,13 +4058,13 @@
         <v>530</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>538</v>
+        <v>582</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1094</v>
       </c>
@@ -4189,7 +4084,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1093</v>
       </c>
@@ -4209,7 +4104,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1068</v>
       </c>
@@ -4226,7 +4121,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1682</v>
       </c>
@@ -4243,7 +4138,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1432</v>
       </c>
@@ -4260,7 +4155,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1239</v>
       </c>
@@ -4277,7 +4172,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>1521</v>
       </c>
@@ -4297,7 +4192,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1221</v>
       </c>
@@ -4410,7 +4305,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1233</v>
       </c>
@@ -4430,7 +4325,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1234</v>
       </c>
@@ -4450,7 +4345,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1235</v>
       </c>
@@ -4470,7 +4365,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1236</v>
       </c>
@@ -4490,7 +4385,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>1232</v>
       </c>
@@ -4507,7 +4402,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>1429</v>
       </c>
@@ -4527,7 +4422,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>1431</v>
       </c>
@@ -4547,7 +4442,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>1430</v>
       </c>
@@ -4567,7 +4462,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>1238</v>
       </c>
@@ -4587,7 +4482,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>1237</v>
       </c>
@@ -4604,7 +4499,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>1611</v>
       </c>
@@ -4624,7 +4519,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>1230</v>
       </c>
@@ -4644,7 +4539,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1229</v>
       </c>
@@ -4661,7 +4556,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>1522</v>
       </c>
@@ -4687,14 +4582,8 @@
         <v>560</v>
       </c>
       <c r="K73" s="6"/>
-      <c r="L73" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M73" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>1225</v>
       </c>
@@ -4720,14 +4609,8 @@
         <v>560</v>
       </c>
       <c r="K74" s="6"/>
-      <c r="L74" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M74" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>1226</v>
       </c>
@@ -4753,14 +4636,8 @@
         <v>560</v>
       </c>
       <c r="K75" s="6"/>
-      <c r="L75" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>1610</v>
       </c>
@@ -4786,14 +4663,8 @@
         <v>560</v>
       </c>
       <c r="K76" s="6"/>
-      <c r="L76" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M76" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>1228</v>
       </c>
@@ -4817,7 +4688,7 @@
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>1428</v>
       </c>
@@ -4843,14 +4714,8 @@
         <v>560</v>
       </c>
       <c r="K78" s="6"/>
-      <c r="L78" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M78" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>1224</v>
       </c>
@@ -4873,14 +4738,8 @@
         <v>560</v>
       </c>
       <c r="K79" s="6"/>
-      <c r="L79" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>1504</v>
       </c>
@@ -4903,7 +4762,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>1505</v>
       </c>
@@ -4926,7 +4785,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>1503</v>
       </c>
@@ -4946,7 +4805,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>1502</v>
       </c>
@@ -4966,7 +4825,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>1601</v>
       </c>
@@ -4986,7 +4845,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>1602</v>
       </c>
@@ -5006,7 +4865,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>1600</v>
       </c>
@@ -5026,7 +4885,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>1459</v>
       </c>
@@ -5046,7 +4905,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>1599</v>
       </c>
@@ -5066,7 +4925,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>1458</v>
       </c>
@@ -5086,7 +4945,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>1457</v>
       </c>
@@ -5106,7 +4965,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>1462</v>
       </c>
@@ -5129,7 +4988,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>1463</v>
       </c>
@@ -5152,7 +5011,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>1461</v>
       </c>
@@ -5172,7 +5031,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>1154</v>
       </c>
@@ -5192,7 +5051,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>1456</v>
       </c>
@@ -5212,7 +5071,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>1460</v>
       </c>
@@ -5232,7 +5091,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>1603</v>
       </c>
@@ -5252,7 +5111,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>1160</v>
       </c>
@@ -5275,7 +5134,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>1475</v>
       </c>
@@ -5298,7 +5157,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>1159</v>
       </c>
@@ -5318,7 +5177,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>1163</v>
       </c>
@@ -5341,7 +5200,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>1162</v>
       </c>
@@ -5364,7 +5223,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>1161</v>
       </c>
@@ -5384,7 +5243,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>1507</v>
       </c>
@@ -5404,7 +5263,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>1578</v>
       </c>
@@ -5430,7 +5289,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>1579</v>
       </c>
@@ -5456,7 +5315,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>1580</v>
       </c>
@@ -5482,7 +5341,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>1581</v>
       </c>
@@ -5508,7 +5367,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>1582</v>
       </c>
@@ -5534,7 +5393,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>1156</v>
       </c>
@@ -5557,7 +5416,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>1157</v>
       </c>
@@ -5580,7 +5439,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>1155</v>
       </c>
@@ -5600,7 +5459,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>1508</v>
       </c>
@@ -5620,7 +5479,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>1604</v>
       </c>
@@ -5652,7 +5511,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>1506</v>
       </c>
@@ -5684,7 +5543,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>1158</v>
       </c>
@@ -5713,7 +5572,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>1165</v>
       </c>
@@ -5736,7 +5595,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>1164</v>
       </c>
@@ -5756,7 +5615,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>1136</v>
       </c>
@@ -5773,7 +5632,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>1138</v>
       </c>
@@ -5793,7 +5652,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>1474</v>
       </c>
@@ -5813,7 +5672,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>1140</v>
       </c>
@@ -5833,7 +5692,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>1141</v>
       </c>
@@ -5853,7 +5712,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>1139</v>
       </c>
@@ -5873,7 +5732,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>1134</v>
       </c>
@@ -5890,7 +5749,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>1605</v>
       </c>
@@ -5913,7 +5772,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>1606</v>
       </c>
@@ -5936,7 +5795,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>1513</v>
       </c>
@@ -5959,7 +5818,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>1512</v>
       </c>
@@ -5982,7 +5841,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>1511</v>
       </c>
@@ -6002,7 +5861,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>1510</v>
       </c>
@@ -6022,7 +5881,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>1509</v>
       </c>
@@ -6042,7 +5901,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>1191</v>
       </c>
@@ -6062,7 +5921,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>1400</v>
       </c>
@@ -6082,7 +5941,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>1190</v>
       </c>
@@ -6102,7 +5961,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>1137</v>
       </c>
@@ -6119,7 +5978,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>1142</v>
       </c>
@@ -6139,7 +5998,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>1143</v>
       </c>
@@ -6159,7 +6018,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>1501</v>
       </c>
@@ -6179,7 +6038,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>1135</v>
       </c>
@@ -6196,7 +6055,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>1666</v>
       </c>
@@ -6216,7 +6075,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>1367</v>
       </c>
@@ -6236,7 +6095,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>1560</v>
       </c>
@@ -6256,7 +6115,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>1366</v>
       </c>
@@ -6276,7 +6135,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>1364</v>
       </c>
@@ -6293,7 +6152,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>1662</v>
       </c>
@@ -6316,7 +6175,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>1663</v>
       </c>
@@ -6342,7 +6201,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>1554</v>
       </c>
@@ -6365,7 +6224,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>1555</v>
       </c>
@@ -6388,7 +6247,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>1553</v>
       </c>
@@ -6408,7 +6267,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>1664</v>
       </c>
@@ -6428,7 +6287,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>1403</v>
       </c>
@@ -6448,7 +6307,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>1665</v>
       </c>
@@ -6468,7 +6327,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>1556</v>
       </c>
@@ -6488,7 +6347,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>1681</v>
       </c>
@@ -6514,7 +6373,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>1349</v>
       </c>
@@ -6537,7 +6396,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>1350</v>
       </c>
@@ -6560,7 +6419,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>1551</v>
       </c>
@@ -6580,7 +6439,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>1557</v>
       </c>
@@ -6600,7 +6459,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>1402</v>
       </c>
@@ -6623,7 +6482,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>1351</v>
       </c>
@@ -6646,7 +6505,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>1352</v>
       </c>
@@ -6669,7 +6528,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>1353</v>
       </c>
@@ -6692,7 +6551,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>1552</v>
       </c>
@@ -6712,7 +6571,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>1348</v>
       </c>
@@ -6729,7 +6588,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>1558</v>
       </c>
@@ -6749,7 +6608,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>1559</v>
       </c>
@@ -6769,7 +6628,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>1548</v>
       </c>
@@ -6789,7 +6648,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>1667</v>
       </c>
@@ -6809,7 +6668,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>1345</v>
       </c>
@@ -6832,7 +6691,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>1344</v>
       </c>
@@ -6855,7 +6714,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>1454</v>
       </c>
@@ -6875,7 +6734,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>1680</v>
       </c>
@@ -6895,7 +6754,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>1625</v>
       </c>
@@ -6915,7 +6774,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>1455</v>
       </c>
@@ -6935,7 +6794,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>1452</v>
       </c>
@@ -6955,7 +6814,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>1549</v>
       </c>
@@ -6975,7 +6834,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>1550</v>
       </c>
@@ -6995,7 +6854,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>1453</v>
       </c>
@@ -7015,7 +6874,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>1660</v>
       </c>
@@ -7035,7 +6894,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>1661</v>
       </c>
@@ -7055,7 +6914,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>1332</v>
       </c>
@@ -7078,7 +6937,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>1330</v>
       </c>
@@ -7101,7 +6960,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>1331</v>
       </c>
@@ -7124,7 +6983,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>1446</v>
       </c>
@@ -7144,7 +7003,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>1546</v>
       </c>
@@ -7167,7 +7026,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>1328</v>
       </c>
@@ -7190,7 +7049,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>1327</v>
       </c>
@@ -7213,7 +7072,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>1445</v>
       </c>
@@ -7233,7 +7092,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>1339</v>
       </c>
@@ -7256,7 +7115,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>1340</v>
       </c>
@@ -7279,7 +7138,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>1451</v>
       </c>
@@ -7299,7 +7158,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>1450</v>
       </c>
@@ -7319,7 +7178,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>1658</v>
       </c>
@@ -7342,7 +7201,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>1438</v>
       </c>
@@ -7365,7 +7224,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>1449</v>
       </c>
@@ -7385,7 +7244,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>1448</v>
       </c>
@@ -7405,7 +7264,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>1447</v>
       </c>
@@ -7425,7 +7284,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>1386</v>
       </c>
@@ -7445,7 +7304,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>1385</v>
       </c>
@@ -7465,7 +7324,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>1668</v>
       </c>
@@ -7485,7 +7344,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>1670</v>
       </c>
@@ -7508,7 +7367,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>1671</v>
       </c>
@@ -7531,7 +7390,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>1669</v>
       </c>
@@ -7551,7 +7410,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>1562</v>
       </c>
@@ -7571,7 +7430,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>1387</v>
       </c>
@@ -7591,7 +7450,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>1563</v>
       </c>
@@ -7611,7 +7470,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>1374</v>
       </c>
@@ -7628,7 +7487,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>1564</v>
       </c>
@@ -7645,7 +7504,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>1482</v>
       </c>
@@ -7662,7 +7521,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>1480</v>
       </c>
@@ -7690,14 +7549,8 @@
       <c r="J211" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L211" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M211" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>1481</v>
       </c>
@@ -7725,14 +7578,8 @@
       <c r="J212" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L212" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M212" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>1383</v>
       </c>
@@ -7757,14 +7604,8 @@
       <c r="J213" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L213" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M213" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>1561</v>
       </c>
@@ -7786,14 +7627,8 @@
       <c r="J214" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L214" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M214" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>1384</v>
       </c>
@@ -7818,14 +7653,8 @@
       <c r="J215" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L215" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M215" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>1382</v>
       </c>
@@ -7850,14 +7679,8 @@
       <c r="J216" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L216" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M216" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>1381</v>
       </c>
@@ -7882,14 +7705,8 @@
       <c r="J217" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L217" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M217" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>1376</v>
       </c>
@@ -7917,14 +7734,8 @@
       <c r="J218" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L218" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M218" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>1379</v>
       </c>
@@ -7952,14 +7763,8 @@
       <c r="J219" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L219" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M219" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>1380</v>
       </c>
@@ -7987,14 +7792,8 @@
       <c r="J220" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L220" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M220" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>1377</v>
       </c>
@@ -8022,14 +7821,8 @@
       <c r="J221" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L221" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M221" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>1378</v>
       </c>
@@ -8057,14 +7850,8 @@
       <c r="J222" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L222" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M222" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>1372</v>
       </c>
@@ -8089,14 +7876,8 @@
       <c r="J223" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L223" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M223" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>1373</v>
       </c>
@@ -8113,7 +7894,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>1371</v>
       </c>
@@ -8130,7 +7911,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>1678</v>
       </c>
@@ -8150,7 +7931,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>1574</v>
       </c>
@@ -8170,7 +7951,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>1442</v>
       </c>
@@ -8190,7 +7971,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>1566</v>
       </c>
@@ -8210,7 +7991,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>1677</v>
       </c>
@@ -8230,7 +8011,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>1440</v>
       </c>
@@ -8250,7 +8031,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>1572</v>
       </c>
@@ -8270,7 +8051,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>1657</v>
       </c>
@@ -8287,7 +8068,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>1576</v>
       </c>
@@ -8307,7 +8088,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>1675</v>
       </c>
@@ -8327,7 +8108,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>1441</v>
       </c>
@@ -8347,7 +8128,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>1443</v>
       </c>
@@ -8367,7 +8148,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>1577</v>
       </c>
@@ -8387,7 +8168,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>1676</v>
       </c>
@@ -8407,7 +8188,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>1575</v>
       </c>
@@ -8427,7 +8208,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>1439</v>
       </c>
@@ -8452,14 +8233,8 @@
       <c r="J241" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="L241" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M241" s="1" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>1567</v>
       </c>
@@ -8479,7 +8254,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>1568</v>
       </c>
@@ -8499,7 +8274,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>1569</v>
       </c>
@@ -8519,7 +8294,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>1570</v>
       </c>
@@ -8539,7 +8314,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>1571</v>
       </c>
@@ -8562,7 +8337,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>1573</v>
       </c>
@@ -8585,7 +8360,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>1674</v>
       </c>
@@ -8605,7 +8380,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>1313</v>
       </c>
@@ -8630,14 +8405,8 @@
       <c r="J249" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L249" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M249" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>1534</v>
       </c>
@@ -8662,14 +8431,11 @@
       <c r="J250" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L250" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="M250" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N250" s="6" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>1533</v>
       </c>
@@ -8697,14 +8463,8 @@
       <c r="J251" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L251" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M251" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>1312</v>
       </c>
@@ -8732,14 +8492,8 @@
       <c r="J252" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L252" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M252" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>1532</v>
       </c>
@@ -8764,14 +8518,8 @@
       <c r="J253" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L253" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M253" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>1476</v>
       </c>
@@ -8796,14 +8544,8 @@
       <c r="J254" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L254" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M254" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>1535</v>
       </c>
@@ -8828,14 +8570,8 @@
       <c r="J255" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L255" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M255" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>1536</v>
       </c>
@@ -8860,14 +8596,8 @@
       <c r="J256" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L256" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M256" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>1311</v>
       </c>
@@ -8892,14 +8622,8 @@
       <c r="J257" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L257" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M257" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>1294</v>
       </c>
@@ -8921,14 +8645,8 @@
       <c r="J258" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L258" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M258" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>1308</v>
       </c>
@@ -8948,7 +8666,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>1617</v>
       </c>
@@ -8968,7 +8686,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>1309</v>
       </c>
@@ -8988,7 +8706,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>1310</v>
       </c>
@@ -9008,7 +8726,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>1293</v>
       </c>
@@ -9025,7 +8743,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>1407</v>
       </c>
@@ -9042,7 +8760,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>1629</v>
       </c>
@@ -9065,7 +8783,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>1627</v>
       </c>
@@ -9088,7 +8806,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>1630</v>
       </c>
@@ -9111,7 +8829,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>1628</v>
       </c>
@@ -9134,7 +8852,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>1626</v>
       </c>
@@ -9157,7 +8875,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>1655</v>
       </c>
@@ -9183,7 +8901,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>1656</v>
       </c>
@@ -9209,7 +8927,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>1654</v>
       </c>
@@ -9232,7 +8950,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>1653</v>
       </c>
@@ -9258,7 +8976,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>1652</v>
       </c>
@@ -9284,7 +9002,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>1651</v>
       </c>
@@ -9307,7 +9025,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>1648</v>
       </c>
@@ -9330,7 +9048,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>1650</v>
       </c>
@@ -9353,7 +9071,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>1647</v>
       </c>
@@ -9376,7 +9094,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <v>1649</v>
       </c>
@@ -9399,7 +9117,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>1631</v>
       </c>
@@ -9422,7 +9140,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>1639</v>
       </c>
@@ -9445,7 +9163,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>1635</v>
       </c>
@@ -9471,7 +9189,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>1636</v>
       </c>
@@ -9497,7 +9215,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>1637</v>
       </c>
@@ -9523,7 +9241,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>1634</v>
       </c>
@@ -9546,7 +9264,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>1638</v>
       </c>
@@ -9569,7 +9287,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>1632</v>
       </c>
@@ -9592,7 +9310,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>1640</v>
       </c>
@@ -9615,7 +9333,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>1633</v>
       </c>
@@ -9638,7 +9356,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>1644</v>
       </c>
@@ -9661,7 +9379,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>1645</v>
       </c>
@@ -9684,7 +9402,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>1646</v>
       </c>
@@ -9707,7 +9425,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>1538</v>
       </c>
@@ -9732,14 +9450,8 @@
       <c r="J293" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L293" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M293" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>1466</v>
       </c>
@@ -9764,14 +9476,8 @@
       <c r="J294" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L294" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M294" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>1465</v>
       </c>
@@ -9796,14 +9502,8 @@
       <c r="J295" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L295" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M295" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>1537</v>
       </c>
@@ -9831,14 +9531,8 @@
       <c r="J296" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L296" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M296" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="297" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>1467</v>
       </c>
@@ -9857,14 +9551,8 @@
       <c r="H297" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="L297" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M297" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="298" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>1477</v>
       </c>
@@ -9889,14 +9577,8 @@
       <c r="J298" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L298" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M298" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>1464</v>
       </c>
@@ -9921,14 +9603,8 @@
       <c r="J299" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L299" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M299" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>1295</v>
       </c>
@@ -9944,14 +9620,8 @@
       <c r="H300" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="L300" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M300" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>1541</v>
       </c>
@@ -9974,7 +9644,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>1544</v>
       </c>
@@ -9997,7 +9667,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>1542</v>
       </c>
@@ -10022,14 +9692,8 @@
       <c r="J303" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="L303" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M303" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="304" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>1406</v>
       </c>
@@ -10049,7 +9713,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
         <v>1322</v>
       </c>
@@ -10069,7 +9733,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <v>1540</v>
       </c>
@@ -10089,7 +9753,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <v>1624</v>
       </c>
@@ -10115,7 +9779,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>1620</v>
       </c>
@@ -10138,7 +9802,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>1623</v>
       </c>
@@ -10164,7 +9828,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>1622</v>
       </c>
@@ -10187,7 +9851,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <v>1621</v>
       </c>
@@ -10210,7 +9874,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <v>1619</v>
       </c>
@@ -10233,7 +9897,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>1618</v>
       </c>
@@ -10253,7 +9917,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>1297</v>
       </c>
@@ -10270,7 +9934,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>1478</v>
       </c>
@@ -10290,7 +9954,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>1545</v>
       </c>
@@ -10307,7 +9971,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <v>1613</v>
       </c>
@@ -10327,7 +9991,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>1278</v>
       </c>
@@ -10347,7 +10011,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>1276</v>
       </c>
@@ -10367,7 +10031,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <v>1529</v>
       </c>
@@ -10387,7 +10051,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <v>1274</v>
       </c>
@@ -10407,7 +10071,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>1279</v>
       </c>
@@ -10427,7 +10091,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>1277</v>
       </c>
@@ -10447,7 +10111,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <v>1530</v>
       </c>
@@ -10467,7 +10131,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <v>1435</v>
       </c>
@@ -10487,7 +10151,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <v>1528</v>
       </c>
@@ -10510,7 +10174,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <v>1282</v>
       </c>
@@ -10533,7 +10197,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>1281</v>
       </c>
@@ -10556,7 +10220,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <v>1527</v>
       </c>
@@ -10579,7 +10243,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>1275</v>
       </c>
@@ -10599,7 +10263,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <v>1242</v>
       </c>
@@ -10616,7 +10280,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2">
         <v>1266</v>
       </c>
@@ -10636,7 +10300,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2">
         <v>1394</v>
       </c>
@@ -10656,7 +10320,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2">
         <v>1267</v>
       </c>
@@ -10676,7 +10340,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2">
         <v>1240</v>
       </c>
@@ -10693,7 +10357,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2">
         <v>1433</v>
       </c>
@@ -10713,7 +10377,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <v>1263</v>
       </c>
@@ -10745,7 +10409,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <v>1259</v>
       </c>
@@ -10777,7 +10441,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <v>1261</v>
       </c>
@@ -10809,7 +10473,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>1260</v>
       </c>
@@ -10841,7 +10505,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <v>1397</v>
       </c>
@@ -10873,7 +10537,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <v>1262</v>
       </c>
@@ -10905,7 +10569,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <v>1258</v>
       </c>
@@ -10931,7 +10595,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <v>1250</v>
       </c>
@@ -10960,7 +10624,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <v>1523</v>
       </c>
@@ -10989,7 +10653,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <v>1249</v>
       </c>
@@ -11015,7 +10679,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <v>1264</v>
       </c>
@@ -11040,14 +10704,8 @@
       <c r="J347" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="L347" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M347" s="1" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <v>1245</v>
       </c>
@@ -11070,7 +10728,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <v>1246</v>
       </c>
@@ -11093,7 +10751,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <v>1247</v>
       </c>
@@ -11116,7 +10774,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <v>1248</v>
       </c>
@@ -11139,7 +10797,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <v>1244</v>
       </c>
@@ -11185,7 +10843,7 @@
         <v>568</v>
       </c>
       <c r="L353" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="M353" s="1" t="s">
         <v>568</v>
@@ -11193,7 +10851,7 @@
       <c r="P353" s="8"/>
       <c r="Q353" s="8"/>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <v>1525</v>
       </c>
@@ -11218,7 +10876,7 @@
       <c r="P354" s="8"/>
       <c r="Q354" s="8"/>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <v>1683</v>
       </c>
@@ -11243,7 +10901,7 @@
       <c r="P355" s="8"/>
       <c r="Q355" s="8"/>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <v>1436</v>
       </c>
@@ -11268,7 +10926,7 @@
       <c r="P356" s="8"/>
       <c r="Q356" s="8"/>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <v>1659</v>
       </c>
@@ -11293,7 +10951,7 @@
       <c r="P357" s="8"/>
       <c r="Q357" s="8"/>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <v>1437</v>
       </c>
@@ -11318,7 +10976,7 @@
       <c r="P358" s="8"/>
       <c r="Q358" s="8"/>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <v>1526</v>
       </c>
@@ -11343,7 +11001,7 @@
       <c r="P359" s="8"/>
       <c r="Q359" s="8"/>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>1434</v>
       </c>
@@ -11364,7 +11022,7 @@
       </c>
       <c r="P360" s="8"/>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>1256</v>
       </c>
@@ -11388,7 +11046,7 @@
       </c>
       <c r="P361" s="8"/>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>1468</v>
       </c>
@@ -11412,7 +11070,7 @@
       </c>
       <c r="P362" s="8"/>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <v>1255</v>
       </c>
@@ -11435,7 +11093,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <v>1257</v>
       </c>
@@ -11458,7 +11116,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <v>1254</v>
       </c>
@@ -11478,7 +11136,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <v>1252</v>
       </c>
@@ -11501,7 +11159,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <v>1524</v>
       </c>
@@ -11524,7 +11182,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <v>1251</v>
       </c>
@@ -11544,7 +11202,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2">
         <v>1470</v>
       </c>
@@ -11569,14 +11227,8 @@
       <c r="J369" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L369" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M369" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370" s="2">
         <v>1287</v>
       </c>
@@ -11602,13 +11254,16 @@
         <v>545</v>
       </c>
       <c r="L370" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="M370" s="1" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N370" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="371" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2">
         <v>1290</v>
       </c>
@@ -11637,7 +11292,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2">
         <v>1531</v>
       </c>
@@ -11660,7 +11315,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373" s="2">
         <v>1286</v>
       </c>
@@ -11686,13 +11341,13 @@
         <v>545</v>
       </c>
       <c r="L373" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="M373" s="1" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2">
         <v>1616</v>
       </c>
@@ -11717,14 +11372,8 @@
       <c r="J374" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L374" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M374" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="375" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2">
         <v>1291</v>
       </c>
@@ -11749,14 +11398,8 @@
       <c r="J375" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L375" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M375" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="376" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2">
         <v>1288</v>
       </c>
@@ -11781,14 +11424,8 @@
       <c r="J376" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L376" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M376" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="377" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <v>1615</v>
       </c>
@@ -11813,14 +11450,8 @@
       <c r="J377" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L377" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M377" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="378" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2">
         <v>1469</v>
       </c>
@@ -11845,14 +11476,8 @@
       <c r="J378" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L378" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M378" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="379" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="2">
         <v>1289</v>
       </c>
@@ -11881,7 +11506,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2">
         <v>1614</v>
       </c>
@@ -11906,14 +11531,8 @@
       <c r="J380" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L380" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M380" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="381" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <v>1408</v>
       </c>
@@ -11941,14 +11560,8 @@
       <c r="J381" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L381" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M381" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="382" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <v>1409</v>
       </c>
@@ -11976,14 +11589,8 @@
       <c r="J382" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L382" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M382" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="383" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <v>1410</v>
       </c>
@@ -12011,14 +11618,8 @@
       <c r="J383" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L383" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M383" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="384" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2">
         <v>1243</v>
       </c>
@@ -12040,14 +11641,8 @@
       <c r="J384" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="L384" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M384" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2">
         <v>1202</v>
       </c>
@@ -12067,7 +11662,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2">
         <v>1201</v>
       </c>
@@ -12084,7 +11679,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2">
         <v>1197</v>
       </c>
@@ -12101,7 +11696,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2">
         <v>1607</v>
       </c>
@@ -12127,7 +11722,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2">
         <v>1520</v>
       </c>
@@ -12153,7 +11748,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2">
         <v>1519</v>
       </c>
@@ -12176,7 +11771,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2">
         <v>1609</v>
       </c>
@@ -12202,7 +11797,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2">
         <v>1608</v>
       </c>
@@ -12225,7 +11820,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2">
         <v>1427</v>
       </c>
@@ -12248,7 +11843,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="2">
         <v>1405</v>
       </c>
@@ -12268,7 +11863,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2">
         <v>1518</v>
       </c>
@@ -12288,7 +11883,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2">
         <v>1404</v>
       </c>
@@ -12308,7 +11903,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2">
         <v>1516</v>
       </c>
@@ -12331,7 +11926,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="2">
         <v>1396</v>
       </c>
@@ -12354,7 +11949,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="2">
         <v>1517</v>
       </c>
@@ -12377,7 +11972,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2">
         <v>1207</v>
       </c>
@@ -12397,7 +11992,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="2">
         <v>1210</v>
       </c>
@@ -12417,7 +12012,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="2">
         <v>1214</v>
       </c>
@@ -12437,7 +12032,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2">
         <v>1679</v>
       </c>
@@ -12457,7 +12052,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2">
         <v>1194</v>
       </c>
@@ -12482,14 +12077,11 @@
       <c r="J404" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="L404" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M404" s="1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K404" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="405" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="2">
         <v>1193</v>
       </c>
@@ -12518,7 +12110,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="2">
         <v>1192</v>
       </c>
@@ -12540,14 +12132,11 @@
       <c r="J406" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="L406" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M406" s="1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K406" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="407" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="2">
         <v>1200</v>
       </c>
@@ -12564,7 +12153,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="2">
         <v>1514</v>
       </c>
@@ -12584,7 +12173,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="2">
         <v>1515</v>
       </c>
@@ -12604,7 +12193,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="2">
         <v>1196</v>
       </c>
@@ -12644,13 +12233,13 @@
         <v>525</v>
       </c>
       <c r="L411" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="M411" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="412" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="2">
         <v>1114</v>
       </c>
@@ -12671,12 +12260,6 @@
       </c>
       <c r="J412" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="L412" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M412" s="1" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="413" spans="1:13" x14ac:dyDescent="0.25">
@@ -12702,13 +12285,13 @@
         <v>525</v>
       </c>
       <c r="L413" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="M413" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="2">
         <v>1496</v>
       </c>
@@ -12733,14 +12316,8 @@
       <c r="J414" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="L414" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M414" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="415" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="2">
         <v>1412</v>
       </c>
@@ -12764,12 +12341,6 @@
       </c>
       <c r="J415" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="L415" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M415" s="1" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="416" spans="1:13" x14ac:dyDescent="0.25">
@@ -12798,13 +12369,13 @@
         <v>525</v>
       </c>
       <c r="L416" s="1" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="M416" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="2">
         <v>1113</v>
       </c>
@@ -12826,14 +12397,8 @@
       <c r="J417" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="L417" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="M417" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="418" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="2">
         <v>1499</v>
       </c>
@@ -12856,7 +12421,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="2">
         <v>1421</v>
       </c>
@@ -12879,7 +12444,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="2">
         <v>1420</v>
       </c>
@@ -12902,7 +12467,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="2">
         <v>1597</v>
       </c>
@@ -12925,7 +12490,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="2">
         <v>1500</v>
       </c>
@@ -12948,7 +12513,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="2">
         <v>1415</v>
       </c>
@@ -12968,7 +12533,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="2">
         <v>1416</v>
       </c>
@@ -12991,7 +12556,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="2">
         <v>1417</v>
       </c>
@@ -13014,7 +12579,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="426" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="2">
         <v>1413</v>
       </c>
@@ -13034,7 +12599,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="2">
         <v>1418</v>
       </c>
@@ -13057,7 +12622,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="428" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="2">
         <v>1598</v>
       </c>
@@ -13080,7 +12645,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="429" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="2">
         <v>1419</v>
       </c>
@@ -13103,7 +12668,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="2">
         <v>1414</v>
       </c>
@@ -13123,7 +12688,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="431" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="2">
         <v>1120</v>
       </c>
@@ -13143,7 +12708,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="2">
         <v>1122</v>
       </c>
@@ -13163,7 +12728,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="2">
         <v>1121</v>
       </c>
@@ -13183,7 +12748,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="2">
         <v>1115</v>
       </c>
@@ -13200,7 +12765,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="2">
         <v>1596</v>
       </c>
@@ -13220,7 +12785,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="2">
         <v>1595</v>
       </c>
@@ -13240,7 +12805,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="2">
         <v>1125</v>
       </c>
@@ -13260,7 +12825,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="2">
         <v>1126</v>
       </c>
@@ -13283,7 +12848,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="2">
         <v>1497</v>
       </c>
@@ -13303,7 +12868,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="2">
         <v>1124</v>
       </c>
@@ -13323,7 +12888,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="2">
         <v>1123</v>
       </c>
@@ -13343,7 +12908,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="2">
         <v>1117</v>
       </c>
@@ -13360,7 +12925,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="2">
         <v>1498</v>
       </c>
@@ -13380,7 +12945,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="2">
         <v>1411</v>
       </c>
@@ -13400,7 +12965,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="2">
         <v>1398</v>
       </c>
@@ -13420,7 +12985,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="2">
         <v>1594</v>
       </c>
@@ -13437,7 +13002,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="2">
         <v>99999</v>
       </c>
@@ -13456,7 +13021,13 @@
   <protectedRanges>
     <protectedRange sqref="A1:XFD1" name="AllowFilter"/>
   </protectedRanges>
-  <autoFilter ref="A1:L447"/>
+  <autoFilter ref="A1:Q447">
+    <filterColumn colId="11">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J447">
     <sortCondition ref="B2:B447"/>
     <sortCondition ref="C2:C447"/>

</xml_diff>

<commit_message>
After call with DH/LC/NT, began implementing requested changes - grouped stroke, ischemic heart disease and peripheral vascular disease as CVD. Removed binge alcohol and HTN duration from regression due to collinearity concerns. Moved univariable regression to Table 1.
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="502">
   <si>
     <t>coding</t>
   </si>
@@ -1459,9 +1459,6 @@
   </si>
   <si>
     <t>unclassifiable</t>
-  </si>
-  <si>
-    <t>ischemic coronary disease</t>
   </si>
   <si>
     <t>CVD</t>
@@ -2425,8 +2422,8 @@
   <dimension ref="A1:M447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A370" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H416" sqref="H416"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2461,16 +2458,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -2506,10 +2503,10 @@
         <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2529,10 +2526,10 @@
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2552,10 +2549,10 @@
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2572,10 +2569,10 @@
         <v>9</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -2594,7 +2591,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2611,10 +2608,10 @@
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2634,7 +2631,7 @@
         <v>479</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -2656,7 +2653,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -2692,13 +2689,13 @@
         <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2718,10 +2715,10 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -2833,7 +2830,7 @@
         <v>479</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -2850,7 +2847,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -3254,10 +3251,10 @@
         <v>51</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -3277,10 +3274,10 @@
         <v>52</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -3297,10 +3294,10 @@
         <v>50</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3333,10 +3330,10 @@
         <v>54</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -3350,10 +3347,10 @@
         <v>49</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>49</v>
+        <v>479</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -3489,7 +3486,7 @@
         <v>62</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -3509,7 +3506,7 @@
         <v>62</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -3526,7 +3523,7 @@
         <v>62</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -4458,7 +4455,7 @@
         <v>125</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
@@ -4480,7 +4477,7 @@
         <v>126</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
@@ -4499,7 +4496,7 @@
         <v>124</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
@@ -6096,7 +6093,7 @@
       <c r="H211" s="1"/>
       <c r="I211" s="1"/>
       <c r="J211" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -6738,7 +6735,7 @@
       <c r="H250" s="1"/>
       <c r="I250" s="1"/>
       <c r="J250" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -7563,7 +7560,7 @@
       <c r="H295" s="1"/>
       <c r="I295" s="1"/>
       <c r="J295" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -7662,7 +7659,7 @@
       <c r="H301" s="1"/>
       <c r="I301" s="1"/>
       <c r="J301" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -7681,7 +7678,7 @@
       <c r="H302" s="1"/>
       <c r="I302" s="1"/>
       <c r="J302" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -8269,7 +8266,7 @@
         <v>365</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H337" s="1"/>
       <c r="I337" s="1"/>
@@ -8291,7 +8288,7 @@
         <v>366</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H338" s="1"/>
       <c r="I338" s="1"/>
@@ -8313,7 +8310,7 @@
         <v>367</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H339" s="1"/>
       <c r="I339" s="1"/>
@@ -8335,7 +8332,7 @@
         <v>368</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H340" s="1"/>
       <c r="I340" s="1"/>
@@ -8357,7 +8354,7 @@
         <v>369</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H341" s="1"/>
       <c r="I341" s="1"/>
@@ -8379,7 +8376,7 @@
         <v>370</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H342" s="1"/>
       <c r="I342" s="1"/>
@@ -8471,7 +8468,7 @@
         <v>374</v>
       </c>
       <c r="I347" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -8583,7 +8580,7 @@
         <v>380</v>
       </c>
       <c r="I353" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
@@ -8909,13 +8906,13 @@
         <v>397</v>
       </c>
       <c r="H370" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I370" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J370" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -8932,7 +8929,7 @@
         <v>398</v>
       </c>
       <c r="G371" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H371" s="1"/>
       <c r="I371" s="1"/>
@@ -8970,10 +8967,10 @@
         <v>399</v>
       </c>
       <c r="H373" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I373" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -9070,7 +9067,7 @@
         <v>406</v>
       </c>
       <c r="G379" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H379" s="1"/>
       <c r="I379" s="1"/>
@@ -9089,10 +9086,10 @@
         <v>407</v>
       </c>
       <c r="H380" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I380" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.3">
@@ -9112,10 +9109,10 @@
         <v>409</v>
       </c>
       <c r="H381" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I381" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="I381" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="382" spans="1:10" x14ac:dyDescent="0.3">
@@ -9135,10 +9132,10 @@
         <v>410</v>
       </c>
       <c r="H382" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I382" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="I382" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.3">
@@ -9158,10 +9155,10 @@
         <v>411</v>
       </c>
       <c r="H383" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I383" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="I383" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
@@ -9236,7 +9233,7 @@
         <v>418</v>
       </c>
       <c r="G388" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H388" s="1"/>
       <c r="I388" s="1"/>
@@ -9258,7 +9255,7 @@
         <v>419</v>
       </c>
       <c r="G389" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H389" s="1"/>
       <c r="I389" s="1"/>
@@ -9277,7 +9274,7 @@
         <v>417</v>
       </c>
       <c r="G390" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H390" s="1"/>
       <c r="I390" s="1"/>
@@ -9299,7 +9296,7 @@
         <v>421</v>
       </c>
       <c r="G391" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H391" s="1"/>
       <c r="I391" s="1"/>
@@ -9318,7 +9315,7 @@
         <v>420</v>
       </c>
       <c r="G392" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H392" s="1"/>
       <c r="I392" s="1"/>
@@ -9337,7 +9334,7 @@
         <v>422</v>
       </c>
       <c r="G393" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H393" s="1"/>
       <c r="I393" s="1"/>
@@ -9353,7 +9350,7 @@
         <v>416</v>
       </c>
       <c r="G394" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H394" s="1"/>
       <c r="I394" s="1"/>
@@ -9525,7 +9522,7 @@
         <v>434</v>
       </c>
       <c r="G404" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H404" s="1"/>
       <c r="I404" s="1"/>
@@ -9544,7 +9541,7 @@
         <v>435</v>
       </c>
       <c r="G405" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H405" s="1"/>
       <c r="I405" s="1"/>
@@ -9560,7 +9557,7 @@
         <v>433</v>
       </c>
       <c r="G406" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H406" s="1"/>
       <c r="I406" s="1"/>
@@ -9634,10 +9631,10 @@
         <v>441</v>
       </c>
       <c r="H411" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I411" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -9664,10 +9661,10 @@
         <v>443</v>
       </c>
       <c r="H413" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I413" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
@@ -9716,10 +9713,10 @@
         <v>447</v>
       </c>
       <c r="H416" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I416" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Removed substance abuse from comorbidities
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TEU\APOE on Dementia\Data Management\R_Dataframes_TLA\38358\Organised\Hypertension\Neo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Kdrive\ukb_hypertension\Data Management\R_Dataframes_TLA\38358\Organised\Hypertension\Neo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="NonCancerIllness" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="502">
   <si>
     <t>coding</t>
   </si>
@@ -1464,9 +1464,6 @@
     <t>CVD</t>
   </si>
   <si>
-    <t>substance use</t>
-  </si>
-  <si>
     <t>Psychiatric</t>
   </si>
   <si>
@@ -1500,9 +1497,6 @@
     <t>UKBTapela_HTN_ManuscriptResults_Feedback20200416.docx "Please remove back pain (do not fold into 'other chronic conditions')</t>
   </si>
   <si>
-    <t>20201604 "Is it possible to have anxiety and depression as two separate comorbidity diagnoses"</t>
-  </si>
-  <si>
     <t>Other cardiometabolic</t>
   </si>
   <si>
@@ -1528,6 +1522,12 @@
   </si>
   <si>
     <t>asthma or COPD</t>
+  </si>
+  <si>
+    <t>20200422 remove substance use (on review it is largely comprised of alcohol dependency, which overlaps with other alcohol indicator; also small n, 388 per table 2)</t>
+  </si>
+  <si>
+    <t>20200416 "Is it possible to have anxiety and depression as two separate comorbidity diagnoses"</t>
   </si>
 </sst>
 </file>
@@ -2422,23 +2422,23 @@
   <dimension ref="A1:M447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J373" sqref="J373"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="12" style="5" customWidth="1"/>
-    <col min="3" max="5" width="19.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="19.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="28.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2458,19 +2458,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1425</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1491</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1583</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1086</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1081</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>1083</v>
       </c>
@@ -2591,10 +2591,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1082</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>1074</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>1588</v>
       </c>
@@ -2653,10 +2653,10 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1079</v>
       </c>
@@ -2672,7 +2672,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1471</v>
       </c>
@@ -2689,16 +2689,16 @@
         <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1483</v>
       </c>
@@ -2715,13 +2715,13 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1485</v>
       </c>
@@ -2740,7 +2740,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1486</v>
       </c>
@@ -2759,7 +2759,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1487</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1484</v>
       </c>
@@ -2797,7 +2797,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1077</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1075</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>1076</v>
       </c>
@@ -2847,12 +2847,12 @@
         <v>27</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1587</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1490</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>1586</v>
       </c>
@@ -2915,7 +2915,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>1585</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>1489</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>1488</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>1584</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>1078</v>
       </c>
@@ -3016,7 +3016,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>1426</v>
       </c>
@@ -3032,7 +3032,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>1590</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>1589</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>1080</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>1479</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>1066</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>1473</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>1072</v>
       </c>
@@ -3144,7 +3144,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>1073</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>1065</v>
       </c>
@@ -3173,7 +3173,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>1495</v>
       </c>
@@ -3189,7 +3189,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>1593</v>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>1494</v>
       </c>
@@ -3221,7 +3221,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>1493</v>
       </c>
@@ -3234,7 +3234,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>1591</v>
       </c>
@@ -3254,10 +3254,10 @@
         <v>479</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>1592</v>
       </c>
@@ -3277,10 +3277,10 @@
         <v>479</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>1492</v>
       </c>
@@ -3297,10 +3297,10 @@
         <v>479</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>1088</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>1087</v>
       </c>
@@ -3333,10 +3333,10 @@
         <v>479</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>1067</v>
       </c>
@@ -3350,10 +3350,10 @@
         <v>479</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>1094</v>
       </c>
@@ -3369,7 +3369,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>1093</v>
       </c>
@@ -3385,7 +3385,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>1068</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>1682</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>1432</v>
       </c>
@@ -3424,7 +3424,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>1239</v>
       </c>
@@ -3437,7 +3437,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>1521</v>
       </c>
@@ -3453,7 +3453,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>1221</v>
       </c>
@@ -3469,7 +3469,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>1222</v>
       </c>
@@ -3486,10 +3486,10 @@
         <v>62</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>1223</v>
       </c>
@@ -3506,10 +3506,10 @@
         <v>62</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>1220</v>
       </c>
@@ -3523,10 +3523,10 @@
         <v>62</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>1233</v>
       </c>
@@ -3542,7 +3542,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>1234</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>1235</v>
       </c>
@@ -3574,7 +3574,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>1236</v>
       </c>
@@ -3590,7 +3590,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>1232</v>
       </c>
@@ -3603,7 +3603,7 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>1429</v>
       </c>
@@ -3619,7 +3619,7 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>1431</v>
       </c>
@@ -3635,7 +3635,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>1430</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>1238</v>
       </c>
@@ -3667,7 +3667,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>1237</v>
       </c>
@@ -3680,7 +3680,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>1611</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>1230</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>1229</v>
       </c>
@@ -3725,7 +3725,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>1522</v>
       </c>
@@ -3741,7 +3741,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>1225</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>1226</v>
       </c>
@@ -3773,7 +3773,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>1610</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>1228</v>
       </c>
@@ -3805,7 +3805,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>1428</v>
       </c>
@@ -3821,7 +3821,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>1224</v>
       </c>
@@ -3834,7 +3834,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>1504</v>
       </c>
@@ -3853,7 +3853,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>1505</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>1503</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>1502</v>
       </c>
@@ -3904,7 +3904,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>1601</v>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>1602</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>1600</v>
       </c>
@@ -3952,7 +3952,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>1459</v>
       </c>
@@ -3968,7 +3968,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>1599</v>
       </c>
@@ -3984,7 +3984,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>1458</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>1457</v>
       </c>
@@ -4016,7 +4016,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>1462</v>
       </c>
@@ -4035,7 +4035,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>1463</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>1461</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>1154</v>
       </c>
@@ -4086,7 +4086,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>1456</v>
       </c>
@@ -4102,7 +4102,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>1460</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>1603</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>1160</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>1475</v>
       </c>
@@ -4172,7 +4172,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>1159</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>1163</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>1162</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>1161</v>
       </c>
@@ -4242,7 +4242,7 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>1507</v>
       </c>
@@ -4258,7 +4258,7 @@
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>1578</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>1579</v>
       </c>
@@ -4302,7 +4302,7 @@
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>1580</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>1581</v>
       </c>
@@ -4346,7 +4346,7 @@
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>1582</v>
       </c>
@@ -4368,7 +4368,7 @@
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>1156</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>1157</v>
       </c>
@@ -4406,7 +4406,7 @@
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>1155</v>
       </c>
@@ -4422,7 +4422,7 @@
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>1508</v>
       </c>
@@ -4438,7 +4438,7 @@
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>1604</v>
       </c>
@@ -4455,12 +4455,12 @@
         <v>125</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>1506</v>
       </c>
@@ -4477,12 +4477,12 @@
         <v>126</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>1158</v>
       </c>
@@ -4496,12 +4496,12 @@
         <v>124</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>1165</v>
       </c>
@@ -4520,7 +4520,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>1164</v>
       </c>
@@ -4536,7 +4536,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>1136</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>1138</v>
       </c>
@@ -4565,7 +4565,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>1474</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>1140</v>
       </c>
@@ -4597,7 +4597,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>1141</v>
       </c>
@@ -4613,7 +4613,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>1139</v>
       </c>
@@ -4629,7 +4629,7 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>1134</v>
       </c>
@@ -4642,7 +4642,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>1605</v>
       </c>
@@ -4661,7 +4661,7 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>1606</v>
       </c>
@@ -4680,7 +4680,7 @@
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>1513</v>
       </c>
@@ -4699,7 +4699,7 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>1512</v>
       </c>
@@ -4718,7 +4718,7 @@
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>1511</v>
       </c>
@@ -4734,7 +4734,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>1510</v>
       </c>
@@ -4750,7 +4750,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>1509</v>
       </c>
@@ -4766,7 +4766,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>1191</v>
       </c>
@@ -4782,7 +4782,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>1400</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>1190</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>1137</v>
       </c>
@@ -4827,7 +4827,7 @@
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>1142</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>1143</v>
       </c>
@@ -4859,7 +4859,7 @@
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>1501</v>
       </c>
@@ -4875,7 +4875,7 @@
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>1135</v>
       </c>
@@ -4888,7 +4888,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>1666</v>
       </c>
@@ -4904,7 +4904,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>1367</v>
       </c>
@@ -4920,7 +4920,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>1560</v>
       </c>
@@ -4936,7 +4936,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>1366</v>
       </c>
@@ -4952,7 +4952,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>1364</v>
       </c>
@@ -4965,7 +4965,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>1662</v>
       </c>
@@ -4984,7 +4984,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>1663</v>
       </c>
@@ -5006,7 +5006,7 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>1554</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>1555</v>
       </c>
@@ -5044,7 +5044,7 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>1553</v>
       </c>
@@ -5060,7 +5060,7 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>1664</v>
       </c>
@@ -5076,7 +5076,7 @@
       <c r="H151" s="1"/>
       <c r="I151" s="1"/>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>1403</v>
       </c>
@@ -5092,7 +5092,7 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <v>1665</v>
       </c>
@@ -5108,7 +5108,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>1556</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>1681</v>
       </c>
@@ -5146,7 +5146,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>1349</v>
       </c>
@@ -5165,7 +5165,7 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>1350</v>
       </c>
@@ -5184,7 +5184,7 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>1551</v>
       </c>
@@ -5200,7 +5200,7 @@
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>1557</v>
       </c>
@@ -5216,7 +5216,7 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>1402</v>
       </c>
@@ -5235,7 +5235,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>1351</v>
       </c>
@@ -5254,7 +5254,7 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>1352</v>
       </c>
@@ -5273,7 +5273,7 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
         <v>1353</v>
       </c>
@@ -5292,7 +5292,7 @@
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>1552</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>1348</v>
       </c>
@@ -5321,7 +5321,7 @@
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>1558</v>
       </c>
@@ -5337,7 +5337,7 @@
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>1559</v>
       </c>
@@ -5353,7 +5353,7 @@
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>1548</v>
       </c>
@@ -5369,7 +5369,7 @@
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>1667</v>
       </c>
@@ -5385,7 +5385,7 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>1345</v>
       </c>
@@ -5404,7 +5404,7 @@
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>1344</v>
       </c>
@@ -5423,7 +5423,7 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>1454</v>
       </c>
@@ -5439,7 +5439,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>1680</v>
       </c>
@@ -5455,7 +5455,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>1625</v>
       </c>
@@ -5471,7 +5471,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>1455</v>
       </c>
@@ -5487,7 +5487,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>1452</v>
       </c>
@@ -5503,7 +5503,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5">
         <v>1549</v>
       </c>
@@ -5519,7 +5519,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>1550</v>
       </c>
@@ -5535,7 +5535,7 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>1453</v>
       </c>
@@ -5551,7 +5551,7 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>1660</v>
       </c>
@@ -5567,7 +5567,7 @@
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>1661</v>
       </c>
@@ -5583,7 +5583,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>1332</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>1330</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>1331</v>
       </c>
@@ -5640,7 +5640,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>1446</v>
       </c>
@@ -5656,7 +5656,7 @@
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>1546</v>
       </c>
@@ -5675,7 +5675,7 @@
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>1328</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>1327</v>
       </c>
@@ -5713,7 +5713,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>1445</v>
       </c>
@@ -5729,7 +5729,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>1339</v>
       </c>
@@ -5748,7 +5748,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="5">
         <v>1340</v>
       </c>
@@ -5767,7 +5767,7 @@
       <c r="H191" s="1"/>
       <c r="I191" s="1"/>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>1451</v>
       </c>
@@ -5783,7 +5783,7 @@
       <c r="H192" s="1"/>
       <c r="I192" s="1"/>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5">
         <v>1450</v>
       </c>
@@ -5799,7 +5799,7 @@
       <c r="H193" s="1"/>
       <c r="I193" s="1"/>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>1658</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="H194" s="1"/>
       <c r="I194" s="1"/>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5">
         <v>1438</v>
       </c>
@@ -5837,7 +5837,7 @@
       <c r="H195" s="1"/>
       <c r="I195" s="1"/>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>1449</v>
       </c>
@@ -5853,7 +5853,7 @@
       <c r="H196" s="1"/>
       <c r="I196" s="1"/>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5">
         <v>1448</v>
       </c>
@@ -5869,7 +5869,7 @@
       <c r="H197" s="1"/>
       <c r="I197" s="1"/>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="5">
         <v>1447</v>
       </c>
@@ -5885,7 +5885,7 @@
       <c r="H198" s="1"/>
       <c r="I198" s="1"/>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="5">
         <v>1386</v>
       </c>
@@ -5901,7 +5901,7 @@
       <c r="H199" s="1"/>
       <c r="I199" s="1"/>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="5">
         <v>1385</v>
       </c>
@@ -5917,7 +5917,7 @@
       <c r="H200" s="1"/>
       <c r="I200" s="1"/>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="5">
         <v>1668</v>
       </c>
@@ -5933,7 +5933,7 @@
       <c r="H201" s="1"/>
       <c r="I201" s="1"/>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="5">
         <v>1670</v>
       </c>
@@ -5952,7 +5952,7 @@
       <c r="H202" s="1"/>
       <c r="I202" s="1"/>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="5">
         <v>1671</v>
       </c>
@@ -5971,7 +5971,7 @@
       <c r="H203" s="1"/>
       <c r="I203" s="1"/>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="5">
         <v>1669</v>
       </c>
@@ -5987,7 +5987,7 @@
       <c r="H204" s="1"/>
       <c r="I204" s="1"/>
     </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="5">
         <v>1562</v>
       </c>
@@ -6003,7 +6003,7 @@
       <c r="H205" s="1"/>
       <c r="I205" s="1"/>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="5">
         <v>1387</v>
       </c>
@@ -6019,7 +6019,7 @@
       <c r="H206" s="1"/>
       <c r="I206" s="1"/>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="5">
         <v>1563</v>
       </c>
@@ -6035,7 +6035,7 @@
       <c r="H207" s="1"/>
       <c r="I207" s="1"/>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="5">
         <v>1374</v>
       </c>
@@ -6048,7 +6048,7 @@
       <c r="H208" s="1"/>
       <c r="I208" s="1"/>
     </row>
-    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="5">
         <v>1564</v>
       </c>
@@ -6061,7 +6061,7 @@
       <c r="H209" s="1"/>
       <c r="I209" s="1"/>
     </row>
-    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="5">
         <v>1482</v>
       </c>
@@ -6074,7 +6074,7 @@
       <c r="H210" s="1"/>
       <c r="I210" s="1"/>
     </row>
-    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="5">
         <v>1480</v>
       </c>
@@ -6093,10 +6093,10 @@
       <c r="H211" s="1"/>
       <c r="I211" s="1"/>
       <c r="J211" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="5">
         <v>1481</v>
       </c>
@@ -6115,7 +6115,7 @@
       <c r="H212" s="1"/>
       <c r="I212" s="1"/>
     </row>
-    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="5">
         <v>1383</v>
       </c>
@@ -6131,7 +6131,7 @@
       <c r="H213" s="1"/>
       <c r="I213" s="1"/>
     </row>
-    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="5">
         <v>1561</v>
       </c>
@@ -6147,7 +6147,7 @@
       <c r="H214" s="1"/>
       <c r="I214" s="1"/>
     </row>
-    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="5">
         <v>1384</v>
       </c>
@@ -6163,7 +6163,7 @@
       <c r="H215" s="1"/>
       <c r="I215" s="1"/>
     </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="5">
         <v>1382</v>
       </c>
@@ -6179,7 +6179,7 @@
       <c r="H216" s="1"/>
       <c r="I216" s="1"/>
     </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="5">
         <v>1381</v>
       </c>
@@ -6195,7 +6195,7 @@
       <c r="H217" s="1"/>
       <c r="I217" s="1"/>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="5">
         <v>1376</v>
       </c>
@@ -6214,7 +6214,7 @@
       <c r="H218" s="1"/>
       <c r="I218" s="1"/>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5">
         <v>1379</v>
       </c>
@@ -6233,7 +6233,7 @@
       <c r="H219" s="1"/>
       <c r="I219" s="1"/>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="5">
         <v>1380</v>
       </c>
@@ -6252,7 +6252,7 @@
       <c r="H220" s="1"/>
       <c r="I220" s="1"/>
     </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="5">
         <v>1377</v>
       </c>
@@ -6271,7 +6271,7 @@
       <c r="H221" s="1"/>
       <c r="I221" s="1"/>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="5">
         <v>1378</v>
       </c>
@@ -6290,7 +6290,7 @@
       <c r="H222" s="1"/>
       <c r="I222" s="1"/>
     </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="5">
         <v>1372</v>
       </c>
@@ -6306,7 +6306,7 @@
       <c r="H223" s="1"/>
       <c r="I223" s="1"/>
     </row>
-    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="5">
         <v>1373</v>
       </c>
@@ -6319,7 +6319,7 @@
       <c r="H224" s="1"/>
       <c r="I224" s="1"/>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="5">
         <v>1371</v>
       </c>
@@ -6332,7 +6332,7 @@
       <c r="H225" s="1"/>
       <c r="I225" s="1"/>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="5">
         <v>1678</v>
       </c>
@@ -6348,7 +6348,7 @@
       <c r="H226" s="1"/>
       <c r="I226" s="1"/>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>1574</v>
       </c>
@@ -6364,7 +6364,7 @@
       <c r="H227" s="1"/>
       <c r="I227" s="1"/>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5">
         <v>1442</v>
       </c>
@@ -6380,7 +6380,7 @@
       <c r="H228" s="1"/>
       <c r="I228" s="1"/>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="5">
         <v>1566</v>
       </c>
@@ -6396,7 +6396,7 @@
       <c r="H229" s="1"/>
       <c r="I229" s="1"/>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5">
         <v>1677</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="H230" s="1"/>
       <c r="I230" s="1"/>
     </row>
-    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5">
         <v>1440</v>
       </c>
@@ -6428,7 +6428,7 @@
       <c r="H231" s="1"/>
       <c r="I231" s="1"/>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5">
         <v>1572</v>
       </c>
@@ -6444,7 +6444,7 @@
       <c r="H232" s="1"/>
       <c r="I232" s="1"/>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="5">
         <v>1657</v>
       </c>
@@ -6457,7 +6457,7 @@
       <c r="H233" s="1"/>
       <c r="I233" s="1"/>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="5">
         <v>1576</v>
       </c>
@@ -6473,7 +6473,7 @@
       <c r="H234" s="1"/>
       <c r="I234" s="1"/>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="5">
         <v>1675</v>
       </c>
@@ -6489,7 +6489,7 @@
       <c r="H235" s="1"/>
       <c r="I235" s="1"/>
     </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="5">
         <v>1441</v>
       </c>
@@ -6505,7 +6505,7 @@
       <c r="H236" s="1"/>
       <c r="I236" s="1"/>
     </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5">
         <v>1443</v>
       </c>
@@ -6521,7 +6521,7 @@
       <c r="H237" s="1"/>
       <c r="I237" s="1"/>
     </row>
-    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="5">
         <v>1577</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="H238" s="1"/>
       <c r="I238" s="1"/>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="5">
         <v>1676</v>
       </c>
@@ -6553,7 +6553,7 @@
       <c r="H239" s="1"/>
       <c r="I239" s="1"/>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="5">
         <v>1575</v>
       </c>
@@ -6569,7 +6569,7 @@
       <c r="H240" s="1"/>
       <c r="I240" s="1"/>
     </row>
-    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="5">
         <v>1439</v>
       </c>
@@ -6585,7 +6585,7 @@
       <c r="H241" s="1"/>
       <c r="I241" s="1"/>
     </row>
-    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5">
         <v>1567</v>
       </c>
@@ -6601,7 +6601,7 @@
       <c r="H242" s="1"/>
       <c r="I242" s="1"/>
     </row>
-    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5">
         <v>1568</v>
       </c>
@@ -6617,7 +6617,7 @@
       <c r="H243" s="1"/>
       <c r="I243" s="1"/>
     </row>
-    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5">
         <v>1569</v>
       </c>
@@ -6633,7 +6633,7 @@
       <c r="H244" s="1"/>
       <c r="I244" s="1"/>
     </row>
-    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="5">
         <v>1570</v>
       </c>
@@ -6649,7 +6649,7 @@
       <c r="H245" s="1"/>
       <c r="I245" s="1"/>
     </row>
-    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="5">
         <v>1571</v>
       </c>
@@ -6668,7 +6668,7 @@
       <c r="H246" s="1"/>
       <c r="I246" s="1"/>
     </row>
-    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="5">
         <v>1573</v>
       </c>
@@ -6687,7 +6687,7 @@
       <c r="H247" s="1"/>
       <c r="I247" s="1"/>
     </row>
-    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="5">
         <v>1674</v>
       </c>
@@ -6703,7 +6703,7 @@
       <c r="H248" s="1"/>
       <c r="I248" s="1"/>
     </row>
-    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="5">
         <v>1313</v>
       </c>
@@ -6719,7 +6719,7 @@
       <c r="H249" s="1"/>
       <c r="I249" s="1"/>
     </row>
-    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="5">
         <v>1534</v>
       </c>
@@ -6735,10 +6735,10 @@
       <c r="H250" s="1"/>
       <c r="I250" s="1"/>
       <c r="J250" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="5">
         <v>1533</v>
       </c>
@@ -6757,7 +6757,7 @@
       <c r="H251" s="1"/>
       <c r="I251" s="1"/>
     </row>
-    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="5">
         <v>1312</v>
       </c>
@@ -6776,7 +6776,7 @@
       <c r="H252" s="1"/>
       <c r="I252" s="1"/>
     </row>
-    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="5">
         <v>1532</v>
       </c>
@@ -6792,7 +6792,7 @@
       <c r="H253" s="1"/>
       <c r="I253" s="1"/>
     </row>
-    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="5">
         <v>1476</v>
       </c>
@@ -6808,7 +6808,7 @@
       <c r="H254" s="1"/>
       <c r="I254" s="1"/>
     </row>
-    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="5">
         <v>1535</v>
       </c>
@@ -6824,7 +6824,7 @@
       <c r="H255" s="1"/>
       <c r="I255" s="1"/>
     </row>
-    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="5">
         <v>1536</v>
       </c>
@@ -6840,7 +6840,7 @@
       <c r="H256" s="1"/>
       <c r="I256" s="1"/>
     </row>
-    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="5">
         <v>1311</v>
       </c>
@@ -6856,7 +6856,7 @@
       <c r="H257" s="1"/>
       <c r="I257" s="1"/>
     </row>
-    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="5">
         <v>1294</v>
       </c>
@@ -6869,7 +6869,7 @@
       <c r="H258" s="1"/>
       <c r="I258" s="1"/>
     </row>
-    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="5">
         <v>1308</v>
       </c>
@@ -6885,7 +6885,7 @@
       <c r="H259" s="1"/>
       <c r="I259" s="1"/>
     </row>
-    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="5">
         <v>1617</v>
       </c>
@@ -6901,7 +6901,7 @@
       <c r="H260" s="1"/>
       <c r="I260" s="1"/>
     </row>
-    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="5">
         <v>1309</v>
       </c>
@@ -6917,7 +6917,7 @@
       <c r="H261" s="1"/>
       <c r="I261" s="1"/>
     </row>
-    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="5">
         <v>1310</v>
       </c>
@@ -6933,7 +6933,7 @@
       <c r="H262" s="1"/>
       <c r="I262" s="1"/>
     </row>
-    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="5">
         <v>1293</v>
       </c>
@@ -6946,7 +6946,7 @@
       <c r="H263" s="1"/>
       <c r="I263" s="1"/>
     </row>
-    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="5">
         <v>1407</v>
       </c>
@@ -6959,7 +6959,7 @@
       <c r="H264" s="1"/>
       <c r="I264" s="1"/>
     </row>
-    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="5">
         <v>1629</v>
       </c>
@@ -6978,7 +6978,7 @@
       <c r="H265" s="1"/>
       <c r="I265" s="1"/>
     </row>
-    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="5">
         <v>1627</v>
       </c>
@@ -6997,7 +6997,7 @@
       <c r="H266" s="1"/>
       <c r="I266" s="1"/>
     </row>
-    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="5">
         <v>1630</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="H267" s="1"/>
       <c r="I267" s="1"/>
     </row>
-    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="5">
         <v>1628</v>
       </c>
@@ -7035,7 +7035,7 @@
       <c r="H268" s="1"/>
       <c r="I268" s="1"/>
     </row>
-    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="5">
         <v>1626</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="H269" s="1"/>
       <c r="I269" s="1"/>
     </row>
-    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="5">
         <v>1655</v>
       </c>
@@ -7076,7 +7076,7 @@
       <c r="H270" s="1"/>
       <c r="I270" s="1"/>
     </row>
-    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="5">
         <v>1656</v>
       </c>
@@ -7098,7 +7098,7 @@
       <c r="H271" s="1"/>
       <c r="I271" s="1"/>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="5">
         <v>1654</v>
       </c>
@@ -7117,7 +7117,7 @@
       <c r="H272" s="1"/>
       <c r="I272" s="1"/>
     </row>
-    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="5">
         <v>1653</v>
       </c>
@@ -7139,7 +7139,7 @@
       <c r="H273" s="1"/>
       <c r="I273" s="1"/>
     </row>
-    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="5">
         <v>1652</v>
       </c>
@@ -7161,7 +7161,7 @@
       <c r="H274" s="1"/>
       <c r="I274" s="1"/>
     </row>
-    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="5">
         <v>1651</v>
       </c>
@@ -7180,7 +7180,7 @@
       <c r="H275" s="1"/>
       <c r="I275" s="1"/>
     </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="5">
         <v>1648</v>
       </c>
@@ -7199,7 +7199,7 @@
       <c r="H276" s="1"/>
       <c r="I276" s="1"/>
     </row>
-    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="5">
         <v>1650</v>
       </c>
@@ -7218,7 +7218,7 @@
       <c r="H277" s="1"/>
       <c r="I277" s="1"/>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="5">
         <v>1647</v>
       </c>
@@ -7237,7 +7237,7 @@
       <c r="H278" s="1"/>
       <c r="I278" s="1"/>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="5">
         <v>1649</v>
       </c>
@@ -7256,7 +7256,7 @@
       <c r="H279" s="1"/>
       <c r="I279" s="1"/>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="5">
         <v>1631</v>
       </c>
@@ -7275,7 +7275,7 @@
       <c r="H280" s="1"/>
       <c r="I280" s="1"/>
     </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="5">
         <v>1639</v>
       </c>
@@ -7294,7 +7294,7 @@
       <c r="H281" s="1"/>
       <c r="I281" s="1"/>
     </row>
-    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="5">
         <v>1635</v>
       </c>
@@ -7316,7 +7316,7 @@
       <c r="H282" s="1"/>
       <c r="I282" s="1"/>
     </row>
-    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="5">
         <v>1636</v>
       </c>
@@ -7338,7 +7338,7 @@
       <c r="H283" s="1"/>
       <c r="I283" s="1"/>
     </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="5">
         <v>1637</v>
       </c>
@@ -7360,7 +7360,7 @@
       <c r="H284" s="1"/>
       <c r="I284" s="1"/>
     </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="5">
         <v>1634</v>
       </c>
@@ -7379,7 +7379,7 @@
       <c r="H285" s="1"/>
       <c r="I285" s="1"/>
     </row>
-    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="5">
         <v>1638</v>
       </c>
@@ -7398,7 +7398,7 @@
       <c r="H286" s="1"/>
       <c r="I286" s="1"/>
     </row>
-    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="5">
         <v>1632</v>
       </c>
@@ -7417,7 +7417,7 @@
       <c r="H287" s="1"/>
       <c r="I287" s="1"/>
     </row>
-    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="5">
         <v>1640</v>
       </c>
@@ -7436,7 +7436,7 @@
       <c r="H288" s="1"/>
       <c r="I288" s="1"/>
     </row>
-    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="5">
         <v>1633</v>
       </c>
@@ -7455,7 +7455,7 @@
       <c r="H289" s="1"/>
       <c r="I289" s="1"/>
     </row>
-    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="5">
         <v>1644</v>
       </c>
@@ -7474,7 +7474,7 @@
       <c r="H290" s="1"/>
       <c r="I290" s="1"/>
     </row>
-    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="5">
         <v>1645</v>
       </c>
@@ -7493,7 +7493,7 @@
       <c r="H291" s="1"/>
       <c r="I291" s="1"/>
     </row>
-    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="5">
         <v>1646</v>
       </c>
@@ -7512,7 +7512,7 @@
       <c r="H292" s="1"/>
       <c r="I292" s="1"/>
     </row>
-    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="5">
         <v>1538</v>
       </c>
@@ -7528,7 +7528,7 @@
       <c r="H293" s="1"/>
       <c r="I293" s="1"/>
     </row>
-    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="5">
         <v>1466</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="H294" s="1"/>
       <c r="I294" s="1"/>
     </row>
-    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="5">
         <v>1465</v>
       </c>
@@ -7560,10 +7560,10 @@
       <c r="H295" s="1"/>
       <c r="I295" s="1"/>
       <c r="J295" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="5">
         <v>1537</v>
       </c>
@@ -7582,7 +7582,7 @@
       <c r="H296" s="1"/>
       <c r="I296" s="1"/>
     </row>
-    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="5">
         <v>1467</v>
       </c>
@@ -7598,7 +7598,7 @@
       <c r="H297" s="1"/>
       <c r="I297" s="1"/>
     </row>
-    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="5">
         <v>1477</v>
       </c>
@@ -7614,7 +7614,7 @@
       <c r="H298" s="1"/>
       <c r="I298" s="1"/>
     </row>
-    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="5">
         <v>1464</v>
       </c>
@@ -7630,7 +7630,7 @@
       <c r="H299" s="1"/>
       <c r="I299" s="1"/>
     </row>
-    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="5">
         <v>1295</v>
       </c>
@@ -7643,7 +7643,7 @@
       <c r="H300" s="1"/>
       <c r="I300" s="1"/>
     </row>
-    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="5">
         <v>1541</v>
       </c>
@@ -7659,10 +7659,10 @@
       <c r="H301" s="1"/>
       <c r="I301" s="1"/>
       <c r="J301" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="5">
         <v>1544</v>
       </c>
@@ -7678,10 +7678,10 @@
       <c r="H302" s="1"/>
       <c r="I302" s="1"/>
       <c r="J302" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="5">
         <v>1542</v>
       </c>
@@ -7697,7 +7697,7 @@
       <c r="H303" s="1"/>
       <c r="I303" s="1"/>
     </row>
-    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="5">
         <v>1406</v>
       </c>
@@ -7713,7 +7713,7 @@
       <c r="H304" s="1"/>
       <c r="I304" s="1"/>
     </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="5">
         <v>1322</v>
       </c>
@@ -7729,7 +7729,7 @@
       <c r="H305" s="1"/>
       <c r="I305" s="1"/>
     </row>
-    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="5">
         <v>1540</v>
       </c>
@@ -7745,7 +7745,7 @@
       <c r="H306" s="1"/>
       <c r="I306" s="1"/>
     </row>
-    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="5">
         <v>1624</v>
       </c>
@@ -7767,7 +7767,7 @@
       <c r="H307" s="1"/>
       <c r="I307" s="1"/>
     </row>
-    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="5">
         <v>1620</v>
       </c>
@@ -7786,7 +7786,7 @@
       <c r="H308" s="1"/>
       <c r="I308" s="1"/>
     </row>
-    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="5">
         <v>1623</v>
       </c>
@@ -7808,7 +7808,7 @@
       <c r="H309" s="1"/>
       <c r="I309" s="1"/>
     </row>
-    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
         <v>1622</v>
       </c>
@@ -7827,7 +7827,7 @@
       <c r="H310" s="1"/>
       <c r="I310" s="1"/>
     </row>
-    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="5">
         <v>1621</v>
       </c>
@@ -7846,7 +7846,7 @@
       <c r="H311" s="1"/>
       <c r="I311" s="1"/>
     </row>
-    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="5">
         <v>1619</v>
       </c>
@@ -7865,7 +7865,7 @@
       <c r="H312" s="1"/>
       <c r="I312" s="1"/>
     </row>
-    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="5">
         <v>1618</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="H313" s="1"/>
       <c r="I313" s="1"/>
     </row>
-    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
         <v>1297</v>
       </c>
@@ -7894,7 +7894,7 @@
       <c r="H314" s="1"/>
       <c r="I314" s="1"/>
     </row>
-    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="5">
         <v>1478</v>
       </c>
@@ -7910,7 +7910,7 @@
       <c r="H315" s="1"/>
       <c r="I315" s="1"/>
     </row>
-    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="5">
         <v>1545</v>
       </c>
@@ -7923,7 +7923,7 @@
       <c r="H316" s="1"/>
       <c r="I316" s="1"/>
     </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="5">
         <v>1613</v>
       </c>
@@ -7939,7 +7939,7 @@
       <c r="H317" s="1"/>
       <c r="I317" s="1"/>
     </row>
-    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
         <v>1278</v>
       </c>
@@ -7955,7 +7955,7 @@
       <c r="H318" s="1"/>
       <c r="I318" s="1"/>
     </row>
-    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="5">
         <v>1276</v>
       </c>
@@ -7971,7 +7971,7 @@
       <c r="H319" s="1"/>
       <c r="I319" s="1"/>
     </row>
-    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="5">
         <v>1529</v>
       </c>
@@ -7987,7 +7987,7 @@
       <c r="H320" s="1"/>
       <c r="I320" s="1"/>
     </row>
-    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="5">
         <v>1274</v>
       </c>
@@ -8003,7 +8003,7 @@
       <c r="H321" s="1"/>
       <c r="I321" s="1"/>
     </row>
-    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="5">
         <v>1279</v>
       </c>
@@ -8019,7 +8019,7 @@
       <c r="H322" s="1"/>
       <c r="I322" s="1"/>
     </row>
-    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="5">
         <v>1277</v>
       </c>
@@ -8035,7 +8035,7 @@
       <c r="H323" s="1"/>
       <c r="I323" s="1"/>
     </row>
-    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
         <v>1530</v>
       </c>
@@ -8051,7 +8051,7 @@
       <c r="H324" s="1"/>
       <c r="I324" s="1"/>
     </row>
-    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="5">
         <v>1435</v>
       </c>
@@ -8067,7 +8067,7 @@
       <c r="H325" s="1"/>
       <c r="I325" s="1"/>
     </row>
-    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="5">
         <v>1528</v>
       </c>
@@ -8086,7 +8086,7 @@
       <c r="H326" s="1"/>
       <c r="I326" s="1"/>
     </row>
-    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="5">
         <v>1282</v>
       </c>
@@ -8105,7 +8105,7 @@
       <c r="H327" s="1"/>
       <c r="I327" s="1"/>
     </row>
-    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
         <v>1281</v>
       </c>
@@ -8124,7 +8124,7 @@
       <c r="H328" s="1"/>
       <c r="I328" s="1"/>
     </row>
-    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
         <v>1527</v>
       </c>
@@ -8143,7 +8143,7 @@
       <c r="H329" s="1"/>
       <c r="I329" s="1"/>
     </row>
-    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="5">
         <v>1275</v>
       </c>
@@ -8159,7 +8159,7 @@
       <c r="H330" s="1"/>
       <c r="I330" s="1"/>
     </row>
-    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
         <v>1242</v>
       </c>
@@ -8172,7 +8172,7 @@
       <c r="H331" s="1"/>
       <c r="I331" s="1"/>
     </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
         <v>1266</v>
       </c>
@@ -8188,7 +8188,7 @@
       <c r="H332" s="1"/>
       <c r="I332" s="1"/>
     </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="5">
         <v>1394</v>
       </c>
@@ -8204,7 +8204,7 @@
       <c r="H333" s="1"/>
       <c r="I333" s="1"/>
     </row>
-    <row r="334" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="5">
         <v>1267</v>
       </c>
@@ -8220,7 +8220,7 @@
       <c r="H334" s="1"/>
       <c r="I334" s="1"/>
     </row>
-    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="5">
         <v>1240</v>
       </c>
@@ -8233,7 +8233,7 @@
       <c r="H335" s="1"/>
       <c r="I335" s="1"/>
     </row>
-    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="5">
         <v>1433</v>
       </c>
@@ -8249,7 +8249,7 @@
       <c r="H336" s="1"/>
       <c r="I336" s="1"/>
     </row>
-    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
         <v>1263</v>
       </c>
@@ -8266,12 +8266,12 @@
         <v>365</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H337" s="1"/>
       <c r="I337" s="1"/>
     </row>
-    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
         <v>1259</v>
       </c>
@@ -8288,12 +8288,12 @@
         <v>366</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H338" s="1"/>
       <c r="I338" s="1"/>
     </row>
-    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
         <v>1261</v>
       </c>
@@ -8310,12 +8310,12 @@
         <v>367</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H339" s="1"/>
       <c r="I339" s="1"/>
     </row>
-    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
         <v>1260</v>
       </c>
@@ -8332,12 +8332,12 @@
         <v>368</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H340" s="1"/>
       <c r="I340" s="1"/>
     </row>
-    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
         <v>1397</v>
       </c>
@@ -8354,12 +8354,12 @@
         <v>369</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H341" s="1"/>
       <c r="I341" s="1"/>
     </row>
-    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
         <v>1262</v>
       </c>
@@ -8376,12 +8376,12 @@
         <v>370</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H342" s="1"/>
       <c r="I342" s="1"/>
     </row>
-    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
         <v>1258</v>
       </c>
@@ -8397,7 +8397,7 @@
       <c r="H343" s="1"/>
       <c r="I343" s="1"/>
     </row>
-    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
         <v>1250</v>
       </c>
@@ -8416,7 +8416,7 @@
       <c r="H344" s="1"/>
       <c r="I344" s="1"/>
     </row>
-    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="5">
         <v>1523</v>
       </c>
@@ -8435,7 +8435,7 @@
       <c r="H345" s="1"/>
       <c r="I345" s="1"/>
     </row>
-    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="5">
         <v>1249</v>
       </c>
@@ -8451,7 +8451,7 @@
       <c r="H346" s="1"/>
       <c r="I346" s="1"/>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" s="5">
         <v>1264</v>
       </c>
@@ -8468,10 +8468,10 @@
         <v>374</v>
       </c>
       <c r="I347" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="5">
         <v>1245</v>
       </c>
@@ -8490,7 +8490,7 @@
       <c r="H348" s="1"/>
       <c r="I348" s="1"/>
     </row>
-    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="5">
         <v>1246</v>
       </c>
@@ -8509,7 +8509,7 @@
       <c r="H349" s="1"/>
       <c r="I349" s="1"/>
     </row>
-    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="5">
         <v>1247</v>
       </c>
@@ -8528,7 +8528,7 @@
       <c r="H350" s="1"/>
       <c r="I350" s="1"/>
     </row>
-    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="5">
         <v>1248</v>
       </c>
@@ -8547,7 +8547,7 @@
       <c r="H351" s="1"/>
       <c r="I351" s="1"/>
     </row>
-    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="5">
         <v>1244</v>
       </c>
@@ -8563,7 +8563,7 @@
       <c r="H352" s="1"/>
       <c r="I352" s="1"/>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A353" s="5">
         <v>1265</v>
       </c>
@@ -8580,12 +8580,12 @@
         <v>380</v>
       </c>
       <c r="I353" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L353" s="6"/>
       <c r="M353" s="6"/>
     </row>
-    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="5">
         <v>1525</v>
       </c>
@@ -8606,7 +8606,7 @@
       <c r="L354" s="6"/>
       <c r="M354" s="6"/>
     </row>
-    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="5">
         <v>1683</v>
       </c>
@@ -8627,7 +8627,7 @@
       <c r="L355" s="6"/>
       <c r="M355" s="6"/>
     </row>
-    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="5">
         <v>1436</v>
       </c>
@@ -8648,7 +8648,7 @@
       <c r="L356" s="6"/>
       <c r="M356" s="6"/>
     </row>
-    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="5">
         <v>1659</v>
       </c>
@@ -8669,7 +8669,7 @@
       <c r="L357" s="6"/>
       <c r="M357" s="6"/>
     </row>
-    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="5">
         <v>1437</v>
       </c>
@@ -8690,7 +8690,7 @@
       <c r="L358" s="6"/>
       <c r="M358" s="6"/>
     </row>
-    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="5">
         <v>1526</v>
       </c>
@@ -8711,7 +8711,7 @@
       <c r="L359" s="6"/>
       <c r="M359" s="6"/>
     </row>
-    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="5">
         <v>1434</v>
       </c>
@@ -8728,7 +8728,7 @@
       <c r="I360" s="1"/>
       <c r="L360" s="6"/>
     </row>
-    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="5">
         <v>1256</v>
       </c>
@@ -8748,7 +8748,7 @@
       <c r="I361" s="1"/>
       <c r="L361" s="6"/>
     </row>
-    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="5">
         <v>1468</v>
       </c>
@@ -8768,7 +8768,7 @@
       <c r="I362" s="1"/>
       <c r="L362" s="6"/>
     </row>
-    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="5">
         <v>1255</v>
       </c>
@@ -8787,7 +8787,7 @@
       <c r="H363" s="1"/>
       <c r="I363" s="1"/>
     </row>
-    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="5">
         <v>1257</v>
       </c>
@@ -8806,7 +8806,7 @@
       <c r="H364" s="1"/>
       <c r="I364" s="1"/>
     </row>
-    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="5">
         <v>1254</v>
       </c>
@@ -8822,7 +8822,7 @@
       <c r="H365" s="1"/>
       <c r="I365" s="1"/>
     </row>
-    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="5">
         <v>1252</v>
       </c>
@@ -8841,7 +8841,7 @@
       <c r="H366" s="1"/>
       <c r="I366" s="1"/>
     </row>
-    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="5">
         <v>1524</v>
       </c>
@@ -8860,7 +8860,7 @@
       <c r="H367" s="1"/>
       <c r="I367" s="1"/>
     </row>
-    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="5">
         <v>1251</v>
       </c>
@@ -8876,7 +8876,7 @@
       <c r="H368" s="1"/>
       <c r="I368" s="1"/>
     </row>
-    <row r="369" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="5">
         <v>1470</v>
       </c>
@@ -8892,7 +8892,7 @@
       <c r="H369" s="1"/>
       <c r="I369" s="1"/>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="5">
         <v>1287</v>
       </c>
@@ -8906,16 +8906,16 @@
         <v>397</v>
       </c>
       <c r="H370" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I370" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J370" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="5">
         <v>1290</v>
       </c>
@@ -8929,12 +8929,12 @@
         <v>398</v>
       </c>
       <c r="G371" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H371" s="1"/>
       <c r="I371" s="1"/>
     </row>
-    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="5">
         <v>1531</v>
       </c>
@@ -8953,7 +8953,7 @@
       <c r="H372" s="1"/>
       <c r="I372" s="1"/>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" s="5">
         <v>1286</v>
       </c>
@@ -8967,13 +8967,13 @@
         <v>399</v>
       </c>
       <c r="H373" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I373" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="5">
         <v>1616</v>
       </c>
@@ -8989,7 +8989,7 @@
       <c r="H374" s="7"/>
       <c r="I374" s="1"/>
     </row>
-    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="5">
         <v>1291</v>
       </c>
@@ -9005,7 +9005,7 @@
       <c r="H375" s="1"/>
       <c r="I375" s="1"/>
     </row>
-    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="5">
         <v>1288</v>
       </c>
@@ -9021,7 +9021,7 @@
       <c r="H376" s="1"/>
       <c r="I376" s="1"/>
     </row>
-    <row r="377" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="5">
         <v>1615</v>
       </c>
@@ -9037,7 +9037,7 @@
       <c r="H377" s="1"/>
       <c r="I377" s="1"/>
     </row>
-    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="5">
         <v>1469</v>
       </c>
@@ -9053,7 +9053,7 @@
       <c r="H378" s="1"/>
       <c r="I378" s="1"/>
     </row>
-    <row r="379" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="5">
         <v>1289</v>
       </c>
@@ -9067,12 +9067,12 @@
         <v>406</v>
       </c>
       <c r="G379" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H379" s="1"/>
       <c r="I379" s="1"/>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" s="5">
         <v>1614</v>
       </c>
@@ -9086,13 +9086,13 @@
         <v>407</v>
       </c>
       <c r="H380" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I380" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" s="5">
         <v>1408</v>
       </c>
@@ -9108,14 +9108,11 @@
       <c r="E381" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="H381" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="I381" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J381" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" s="5">
         <v>1409</v>
       </c>
@@ -9131,14 +9128,11 @@
       <c r="E382" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="H382" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="I382" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J382" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
         <v>1410</v>
       </c>
@@ -9154,14 +9148,11 @@
       <c r="E383" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="H383" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="I383" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J383" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="5">
         <v>1243</v>
       </c>
@@ -9174,7 +9165,7 @@
       <c r="H384" s="1"/>
       <c r="I384" s="1"/>
     </row>
-    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="5">
         <v>1202</v>
       </c>
@@ -9190,7 +9181,7 @@
       <c r="H385" s="1"/>
       <c r="I385" s="1"/>
     </row>
-    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="5">
         <v>1201</v>
       </c>
@@ -9203,7 +9194,7 @@
       <c r="H386" s="1"/>
       <c r="I386" s="1"/>
     </row>
-    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="5">
         <v>1197</v>
       </c>
@@ -9216,7 +9207,7 @@
       <c r="H387" s="1"/>
       <c r="I387" s="1"/>
     </row>
-    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="5">
         <v>1607</v>
       </c>
@@ -9233,12 +9224,12 @@
         <v>418</v>
       </c>
       <c r="G388" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H388" s="1"/>
       <c r="I388" s="1"/>
     </row>
-    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="5">
         <v>1520</v>
       </c>
@@ -9255,12 +9246,12 @@
         <v>419</v>
       </c>
       <c r="G389" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H389" s="1"/>
       <c r="I389" s="1"/>
     </row>
-    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="5">
         <v>1519</v>
       </c>
@@ -9274,12 +9265,12 @@
         <v>417</v>
       </c>
       <c r="G390" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H390" s="1"/>
       <c r="I390" s="1"/>
     </row>
-    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="5">
         <v>1609</v>
       </c>
@@ -9296,12 +9287,12 @@
         <v>421</v>
       </c>
       <c r="G391" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H391" s="1"/>
       <c r="I391" s="1"/>
     </row>
-    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="5">
         <v>1608</v>
       </c>
@@ -9315,12 +9306,12 @@
         <v>420</v>
       </c>
       <c r="G392" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H392" s="1"/>
       <c r="I392" s="1"/>
     </row>
-    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="5">
         <v>1427</v>
       </c>
@@ -9334,12 +9325,12 @@
         <v>422</v>
       </c>
       <c r="G393" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H393" s="1"/>
       <c r="I393" s="1"/>
     </row>
-    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="5">
         <v>1405</v>
       </c>
@@ -9350,12 +9341,12 @@
         <v>416</v>
       </c>
       <c r="G394" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H394" s="1"/>
       <c r="I394" s="1"/>
     </row>
-    <row r="395" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="5">
         <v>1518</v>
       </c>
@@ -9371,7 +9362,7 @@
       <c r="H395" s="1"/>
       <c r="I395" s="1"/>
     </row>
-    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="5">
         <v>1404</v>
       </c>
@@ -9387,7 +9378,7 @@
       <c r="H396" s="1"/>
       <c r="I396" s="1"/>
     </row>
-    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="5">
         <v>1516</v>
       </c>
@@ -9406,7 +9397,7 @@
       <c r="H397" s="1"/>
       <c r="I397" s="1"/>
     </row>
-    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="5">
         <v>1396</v>
       </c>
@@ -9425,7 +9416,7 @@
       <c r="H398" s="1"/>
       <c r="I398" s="1"/>
     </row>
-    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="5">
         <v>1517</v>
       </c>
@@ -9444,7 +9435,7 @@
       <c r="H399" s="1"/>
       <c r="I399" s="1"/>
     </row>
-    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="5">
         <v>1207</v>
       </c>
@@ -9460,7 +9451,7 @@
       <c r="H400" s="1"/>
       <c r="I400" s="1"/>
     </row>
-    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="5">
         <v>1210</v>
       </c>
@@ -9476,7 +9467,7 @@
       <c r="H401" s="1"/>
       <c r="I401" s="1"/>
     </row>
-    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="5">
         <v>1214</v>
       </c>
@@ -9492,7 +9483,7 @@
       <c r="H402" s="1"/>
       <c r="I402" s="1"/>
     </row>
-    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="5">
         <v>1679</v>
       </c>
@@ -9508,7 +9499,7 @@
       <c r="H403" s="1"/>
       <c r="I403" s="1"/>
     </row>
-    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
         <v>1194</v>
       </c>
@@ -9522,12 +9513,12 @@
         <v>434</v>
       </c>
       <c r="G404" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H404" s="1"/>
       <c r="I404" s="1"/>
     </row>
-    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="5">
         <v>1193</v>
       </c>
@@ -9541,12 +9532,12 @@
         <v>435</v>
       </c>
       <c r="G405" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H405" s="1"/>
       <c r="I405" s="1"/>
     </row>
-    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="5">
         <v>1192</v>
       </c>
@@ -9557,12 +9548,12 @@
         <v>433</v>
       </c>
       <c r="G406" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H406" s="1"/>
       <c r="I406" s="1"/>
     </row>
-    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="5">
         <v>1200</v>
       </c>
@@ -9575,7 +9566,7 @@
       <c r="H407" s="1"/>
       <c r="I407" s="1"/>
     </row>
-    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="5">
         <v>1514</v>
       </c>
@@ -9591,7 +9582,7 @@
       <c r="H408" s="1"/>
       <c r="I408" s="1"/>
     </row>
-    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="5">
         <v>1515</v>
       </c>
@@ -9607,7 +9598,7 @@
       <c r="H409" s="1"/>
       <c r="I409" s="1"/>
     </row>
-    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="5">
         <v>1196</v>
       </c>
@@ -9620,7 +9611,7 @@
       <c r="H410" s="1"/>
       <c r="I410" s="1"/>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A411" s="5">
         <v>1111</v>
       </c>
@@ -9631,13 +9622,13 @@
         <v>441</v>
       </c>
       <c r="H411" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I411" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" s="5">
         <v>1114</v>
       </c>
@@ -9650,7 +9641,7 @@
       <c r="H412" s="1"/>
       <c r="I412" s="1"/>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A413" s="5">
         <v>1112</v>
       </c>
@@ -9661,13 +9652,13 @@
         <v>443</v>
       </c>
       <c r="H413" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I413" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="5">
         <v>1496</v>
       </c>
@@ -9683,7 +9674,7 @@
       <c r="H414" s="1"/>
       <c r="I414" s="1"/>
     </row>
-    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="5">
         <v>1412</v>
       </c>
@@ -9699,7 +9690,7 @@
       <c r="H415" s="1"/>
       <c r="I415" s="1"/>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A416" s="5">
         <v>1472</v>
       </c>
@@ -9713,13 +9704,13 @@
         <v>447</v>
       </c>
       <c r="H416" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I416" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="5">
         <v>1113</v>
       </c>
@@ -9732,7 +9723,7 @@
       <c r="H417" s="1"/>
       <c r="I417" s="1"/>
     </row>
-    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="5">
         <v>1499</v>
       </c>
@@ -9751,7 +9742,7 @@
       <c r="H418" s="1"/>
       <c r="I418" s="1"/>
     </row>
-    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="5">
         <v>1421</v>
       </c>
@@ -9770,7 +9761,7 @@
       <c r="H419" s="1"/>
       <c r="I419" s="1"/>
     </row>
-    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="5">
         <v>1420</v>
       </c>
@@ -9789,7 +9780,7 @@
       <c r="H420" s="1"/>
       <c r="I420" s="1"/>
     </row>
-    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
         <v>1597</v>
       </c>
@@ -9808,7 +9799,7 @@
       <c r="H421" s="1"/>
       <c r="I421" s="1"/>
     </row>
-    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="5">
         <v>1500</v>
       </c>
@@ -9827,7 +9818,7 @@
       <c r="H422" s="1"/>
       <c r="I422" s="1"/>
     </row>
-    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="5">
         <v>1415</v>
       </c>
@@ -9843,7 +9834,7 @@
       <c r="H423" s="1"/>
       <c r="I423" s="1"/>
     </row>
-    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="5">
         <v>1416</v>
       </c>
@@ -9862,7 +9853,7 @@
       <c r="H424" s="1"/>
       <c r="I424" s="1"/>
     </row>
-    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="5">
         <v>1417</v>
       </c>
@@ -9881,7 +9872,7 @@
       <c r="H425" s="1"/>
       <c r="I425" s="1"/>
     </row>
-    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="5">
         <v>1413</v>
       </c>
@@ -9897,7 +9888,7 @@
       <c r="H426" s="1"/>
       <c r="I426" s="1"/>
     </row>
-    <row r="427" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="5">
         <v>1418</v>
       </c>
@@ -9916,7 +9907,7 @@
       <c r="H427" s="1"/>
       <c r="I427" s="1"/>
     </row>
-    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="5">
         <v>1598</v>
       </c>
@@ -9935,7 +9926,7 @@
       <c r="H428" s="1"/>
       <c r="I428" s="1"/>
     </row>
-    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="5">
         <v>1419</v>
       </c>
@@ -9954,7 +9945,7 @@
       <c r="H429" s="1"/>
       <c r="I429" s="1"/>
     </row>
-    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="5">
         <v>1414</v>
       </c>
@@ -9970,7 +9961,7 @@
       <c r="H430" s="1"/>
       <c r="I430" s="1"/>
     </row>
-    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" s="5">
         <v>1120</v>
       </c>
@@ -9986,7 +9977,7 @@
       <c r="H431" s="1"/>
       <c r="I431" s="1"/>
     </row>
-    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="5">
         <v>1122</v>
       </c>
@@ -10002,7 +9993,7 @@
       <c r="H432" s="1"/>
       <c r="I432" s="1"/>
     </row>
-    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="5">
         <v>1121</v>
       </c>
@@ -10018,7 +10009,7 @@
       <c r="H433" s="1"/>
       <c r="I433" s="1"/>
     </row>
-    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="5">
         <v>1115</v>
       </c>
@@ -10031,7 +10022,7 @@
       <c r="H434" s="1"/>
       <c r="I434" s="1"/>
     </row>
-    <row r="435" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="5">
         <v>1596</v>
       </c>
@@ -10047,7 +10038,7 @@
       <c r="H435" s="1"/>
       <c r="I435" s="1"/>
     </row>
-    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="5">
         <v>1595</v>
       </c>
@@ -10063,7 +10054,7 @@
       <c r="H436" s="1"/>
       <c r="I436" s="1"/>
     </row>
-    <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="5">
         <v>1125</v>
       </c>
@@ -10079,7 +10070,7 @@
       <c r="H437" s="1"/>
       <c r="I437" s="1"/>
     </row>
-    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="5">
         <v>1126</v>
       </c>
@@ -10098,7 +10089,7 @@
       <c r="H438" s="1"/>
       <c r="I438" s="1"/>
     </row>
-    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="5">
         <v>1497</v>
       </c>
@@ -10114,7 +10105,7 @@
       <c r="H439" s="1"/>
       <c r="I439" s="1"/>
     </row>
-    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="5">
         <v>1124</v>
       </c>
@@ -10130,7 +10121,7 @@
       <c r="H440" s="1"/>
       <c r="I440" s="1"/>
     </row>
-    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="5">
         <v>1123</v>
       </c>
@@ -10146,7 +10137,7 @@
       <c r="H441" s="1"/>
       <c r="I441" s="1"/>
     </row>
-    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="5">
         <v>1117</v>
       </c>
@@ -10159,7 +10150,7 @@
       <c r="H442" s="1"/>
       <c r="I442" s="1"/>
     </row>
-    <row r="443" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="5">
         <v>1498</v>
       </c>
@@ -10175,7 +10166,7 @@
       <c r="H443" s="1"/>
       <c r="I443" s="1"/>
     </row>
-    <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" s="5">
         <v>1411</v>
       </c>
@@ -10191,7 +10182,7 @@
       <c r="H444" s="1"/>
       <c r="I444" s="1"/>
     </row>
-    <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" s="5">
         <v>1398</v>
       </c>
@@ -10207,7 +10198,7 @@
       <c r="H445" s="1"/>
       <c r="I445" s="1"/>
     </row>
-    <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" s="5">
         <v>1594</v>
       </c>
@@ -10220,7 +10211,7 @@
       <c r="H446" s="1"/>
       <c r="I446" s="1"/>
     </row>
-    <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" s="5">
         <v>99999</v>
       </c>

</xml_diff>

<commit_message>
New version of comorbidity mapping
</commit_message>
<xml_diff>
--- a/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
+++ b/Data Management/R_Dataframes_TLA/38358/Organised/Hypertension/Neo/UKBHtn_NonCancerIllness_Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Kdrive\ukb_hypertension\Data Management\R_Dataframes_TLA\38358\Organised\Hypertension\Neo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TEU\APOE on Dementia\Data Management\R_Dataframes_TLA\38358\Organised\Hypertension\Neo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="NonCancerIllness" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="505">
   <si>
     <t>coding</t>
   </si>
@@ -1506,9 +1506,6 @@
     <t>ComorbidityCondition</t>
   </si>
   <si>
-    <t>20200417: No longer including arthritis in analysis</t>
-  </si>
-  <si>
     <t>20200417: No longer including systemic connective tissue disorders in analysis</t>
   </si>
   <si>
@@ -1528,6 +1525,18 @@
   </si>
   <si>
     <t>20200416 "Is it possible to have anxiety and depression as two separate comorbidity diagnoses"</t>
+  </si>
+  <si>
+    <t>Osteoarthritis</t>
+  </si>
+  <si>
+    <t>Other joint disorder</t>
+  </si>
+  <si>
+    <t>20200427: arthritis is back in</t>
+  </si>
+  <si>
+    <t>Joint disorders</t>
   </si>
 </sst>
 </file>
@@ -2138,9 +2147,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Neo Tapela" id="{52D97C36-8B99-D14C-BE04-DF229B6C102C}" userId="2323a1ee987b6196" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2404,31 +2411,19 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I1" dT="2020-04-17T07:08:22.18" personId="{52D97C36-8B99-D14C-BE04-DF229B6C102C}" id="{95101964-7067-5B4E-B716-CBB7B4C4B307}">
-    <text>note that this is comorbidity CONDITION</text>
-  </threadedComment>
-  <threadedComment ref="M12" dT="2020-04-17T07:22:48.47" personId="{52D97C36-8B99-D14C-BE04-DF229B6C102C}" id="{FC5F44EA-0D0A-2248-8A7A-FA70152585AF}">
-    <text xml:space="preserve">revised name from ‘other cardiac’
-</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:M447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J373" sqref="J373"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I298" sqref="I298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8" style="5" customWidth="1"/>
     <col min="2" max="2" width="12" style="5" customWidth="1"/>
     <col min="3" max="5" width="19.28515625" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="5" customWidth="1"/>
@@ -2689,7 +2684,7 @@
         <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>491</v>
@@ -2715,7 +2710,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>491</v>
@@ -6093,7 +6088,7 @@
       <c r="H211" s="1"/>
       <c r="I211" s="1"/>
       <c r="J211" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -7512,7 +7507,7 @@
       <c r="H292" s="1"/>
       <c r="I292" s="1"/>
     </row>
-    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="5">
         <v>1538</v>
       </c>
@@ -7525,8 +7520,12 @@
       <c r="D293" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="H293" s="1"/>
-      <c r="I293" s="1"/>
+      <c r="H293" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I293" s="1" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="5">
@@ -7544,7 +7543,7 @@
       <c r="H294" s="1"/>
       <c r="I294" s="1"/>
     </row>
-    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="5">
         <v>1465</v>
       </c>
@@ -7557,13 +7556,17 @@
       <c r="D295" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="H295" s="1"/>
-      <c r="I295" s="1"/>
+      <c r="H295" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I295" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="J295" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="5">
         <v>1537</v>
       </c>
@@ -7579,10 +7582,14 @@
       <c r="E296" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="H296" s="1"/>
-      <c r="I296" s="1"/>
-    </row>
-    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H296" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I296" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="5">
         <v>1467</v>
       </c>
@@ -7595,10 +7602,14 @@
       <c r="D297" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="H297" s="1"/>
-      <c r="I297" s="1"/>
-    </row>
-    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H297" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I297" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="5">
         <v>1477</v>
       </c>
@@ -7611,10 +7622,14 @@
       <c r="D298" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="H298" s="1"/>
-      <c r="I298" s="1"/>
-    </row>
-    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H298" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I298" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="5">
         <v>1464</v>
       </c>
@@ -7627,10 +7642,14 @@
       <c r="D299" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="H299" s="1"/>
-      <c r="I299" s="1"/>
-    </row>
-    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H299" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I299" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="5">
         <v>1295</v>
       </c>
@@ -7640,8 +7659,12 @@
       <c r="C300" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="H300" s="1"/>
-      <c r="I300" s="1"/>
+      <c r="H300" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="I300" s="1" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="5">
@@ -8906,13 +8929,13 @@
         <v>397</v>
       </c>
       <c r="H370" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I370" s="2" t="s">
         <v>480</v>
       </c>
       <c r="J370" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="371" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -8967,7 +8990,7 @@
         <v>399</v>
       </c>
       <c r="H373" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I373" s="2" t="s">
         <v>480</v>
@@ -9086,13 +9109,13 @@
         <v>407</v>
       </c>
       <c r="H380" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I380" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="5">
         <v>1408</v>
       </c>
@@ -9109,10 +9132,10 @@
         <v>409</v>
       </c>
       <c r="J381" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="5">
         <v>1409</v>
       </c>
@@ -9129,10 +9152,10 @@
         <v>410</v>
       </c>
       <c r="J382" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
         <v>1410</v>
       </c>
@@ -9149,7 +9172,7 @@
         <v>411</v>
       </c>
       <c r="J383" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -9622,7 +9645,7 @@
         <v>441</v>
       </c>
       <c r="H411" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I411" s="2" t="s">
         <v>487</v>
@@ -9652,7 +9675,7 @@
         <v>443</v>
       </c>
       <c r="H413" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I413" s="2" t="s">
         <v>487</v>
@@ -9704,7 +9727,7 @@
         <v>447</v>
       </c>
       <c r="H416" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I416" s="2" t="s">
         <v>487</v>
@@ -10243,4 +10266,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051639A54F254114DAFE5D53E0D26CB6A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="513fdb8a5cb2886c5cecc82f266a9aba">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="50bcf86c-e7e7-49ca-8df1-ae74924c9d38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0adb841d0dc2155ad956e5150cf65a20" ns2:_="">
+    <xsd:import namespace="50bcf86c-e7e7-49ca-8df1-ae74924c9d38"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="50bcf86c-e7e7-49ca-8df1-ae74924c9d38" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{287D6A4E-3346-4B71-A978-E0CD331EA814}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="50bcf86c-e7e7-49ca-8df1-ae74924c9d38"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{262424A3-453B-4C99-838E-9CDA4F9635BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8869C1EC-785D-4FDD-A3B2-A2E0E40CB5AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="50bcf86c-e7e7-49ca-8df1-ae74924c9d38"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>